<commit_message>
20 de junho de 2017 - INESC
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/Book1.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marisaoliveira/Desktop/tese/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marisaoliveira/Master-Thesis/mieec-distrib-v2014/outras_cenas/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="915">
   <si>
     <t>I/O</t>
   </si>
@@ -2160,9 +2160,6 @@
     <t>Only sound</t>
   </si>
   <si>
-    <t>Plano D</t>
-  </si>
-  <si>
     <t>Nome da Porta</t>
   </si>
   <si>
@@ -2734,12 +2731,69 @@
   </si>
   <si>
     <t>diz q há cenas para mandar as commas e isso</t>
+  </si>
+  <si>
+    <t>Interface com a FPGA</t>
+  </si>
+  <si>
+    <t>Codificação 8B/10B</t>
+  </si>
+  <si>
+    <t>Tamanho do Datapath</t>
+  </si>
+  <si>
+    <t>Tamanho interno do datapath</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>2 byte</t>
+  </si>
+  <si>
+    <t>4 byte</t>
+  </si>
+  <si>
+    <t>148, 5 MHz</t>
+  </si>
+  <si>
+    <t>148,5 MHz</t>
+  </si>
+  <si>
+    <t>2,97 Gb/s</t>
+  </si>
+  <si>
+    <t>2,376 Gb/s</t>
+  </si>
+  <si>
+    <t>297 MHz</t>
+  </si>
+  <si>
+    <t>5,94 Gb/s</t>
+  </si>
+  <si>
+    <t>4,752 Gb/s</t>
+  </si>
+  <si>
+    <t>11,88 Gb/s</t>
+  </si>
+  <si>
+    <t>9,5 Gb/s</t>
+  </si>
+  <si>
+    <t>Velocidade em série</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3729,7 +3783,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3759,8 +3813,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -4370,6 +4426,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4474,6 +4533,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4504,12 +4569,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4552,8 +4611,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -4570,6 +4660,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
@@ -4580,6 +4671,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -4875,60 +4967,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="223" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
-      <c r="I1" s="222"/>
-      <c r="J1" s="222"/>
-      <c r="K1" s="222"/>
-      <c r="L1" s="222"/>
-      <c r="M1" s="222"/>
-      <c r="N1" s="222"/>
-      <c r="O1" s="222"/>
-      <c r="P1" s="222"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
+      <c r="I1" s="223"/>
+      <c r="J1" s="223"/>
+      <c r="K1" s="223"/>
+      <c r="L1" s="223"/>
+      <c r="M1" s="223"/>
+      <c r="N1" s="223"/>
+      <c r="O1" s="223"/>
+      <c r="P1" s="223"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="222"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
-      <c r="I2" s="222"/>
-      <c r="J2" s="222"/>
-      <c r="K2" s="222"/>
-      <c r="L2" s="222"/>
-      <c r="M2" s="222"/>
-      <c r="N2" s="222"/>
-      <c r="O2" s="222"/>
-      <c r="P2" s="222"/>
+      <c r="A2" s="223"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
+      <c r="I2" s="223"/>
+      <c r="J2" s="223"/>
+      <c r="K2" s="223"/>
+      <c r="L2" s="223"/>
+      <c r="M2" s="223"/>
+      <c r="N2" s="223"/>
+      <c r="O2" s="223"/>
+      <c r="P2" s="223"/>
     </row>
     <row r="3" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="222"/>
-      <c r="B3" s="222"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="222"/>
+      <c r="A3" s="223"/>
+      <c r="B3" s="223"/>
+      <c r="C3" s="223"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
+      <c r="L3" s="223"/>
+      <c r="M3" s="223"/>
+      <c r="N3" s="223"/>
+      <c r="O3" s="223"/>
+      <c r="P3" s="223"/>
     </row>
     <row r="4" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -4961,14 +5053,14 @@
       <c r="K4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="223" t="s">
+      <c r="M4" s="224" t="s">
         <v>196</v>
       </c>
-      <c r="N4" s="224"/>
-      <c r="O4" s="224"/>
-      <c r="P4" s="224"/>
-      <c r="Q4" s="224"/>
-      <c r="R4" s="225"/>
+      <c r="N4" s="225"/>
+      <c r="O4" s="225"/>
+      <c r="P4" s="225"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="226"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5189,14 +5281,14 @@
       <c r="F9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="226" t="s">
+      <c r="M9" s="227" t="s">
         <v>200</v>
       </c>
-      <c r="N9" s="227"/>
-      <c r="O9" s="227"/>
-      <c r="P9" s="227"/>
-      <c r="Q9" s="227"/>
-      <c r="R9" s="228"/>
+      <c r="N9" s="228"/>
+      <c r="O9" s="228"/>
+      <c r="P9" s="228"/>
+      <c r="Q9" s="228"/>
+      <c r="R9" s="229"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -5779,14 +5871,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="229" t="s">
+      <c r="A39" s="230" t="s">
         <v>403</v>
       </c>
-      <c r="B39" s="230"/>
-      <c r="C39" s="230"/>
-      <c r="D39" s="230"/>
-      <c r="E39" s="230"/>
-      <c r="F39" s="231"/>
+      <c r="B39" s="231"/>
+      <c r="C39" s="231"/>
+      <c r="D39" s="231"/>
+      <c r="E39" s="231"/>
+      <c r="F39" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8343,7 +8435,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="272" t="s">
+      <c r="G107" s="273" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -8379,7 +8471,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="273"/>
+      <c r="G108" s="274"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -8417,7 +8509,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="274" t="s">
+      <c r="J109" s="275" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -8445,7 +8537,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="274"/>
+      <c r="J110" s="275"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -8465,7 +8557,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="274"/>
+      <c r="J111" s="275"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -8485,7 +8577,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="274"/>
+      <c r="J112" s="275"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>
@@ -8547,24 +8639,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L20"/>
+  <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B39" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>692</v>
       </c>
@@ -8576,8 +8669,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:12" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="79" t="s">
         <v>702</v>
       </c>
@@ -8606,11 +8699,11 @@
         <v>701</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="281" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="282" t="s">
         <v>703</v>
       </c>
-      <c r="D6" s="279">
+      <c r="D6" s="280">
         <v>64</v>
       </c>
       <c r="E6" s="46">
@@ -8638,9 +8731,9 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="282"/>
-      <c r="D7" s="275"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C7" s="283"/>
+      <c r="D7" s="276"/>
       <c r="E7" s="92">
         <v>1</v>
       </c>
@@ -8666,14 +8759,14 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" s="277" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="278" t="s">
         <v>704</v>
       </c>
-      <c r="D8" s="280">
+      <c r="D8" s="281">
         <v>40</v>
       </c>
-      <c r="E8" s="280">
+      <c r="E8" s="281">
         <v>0</v>
       </c>
       <c r="F8" s="67">
@@ -8697,14 +8790,11 @@
       <c r="K8" s="83">
         <v>5.9</v>
       </c>
-      <c r="L8" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" s="277"/>
-      <c r="D9" s="280"/>
-      <c r="E9" s="280"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C9" s="278"/>
+      <c r="D9" s="281"/>
+      <c r="E9" s="281"/>
       <c r="F9" s="92">
         <v>1</v>
       </c>
@@ -8727,11 +8817,11 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C10" s="277" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="278" t="s">
         <v>705</v>
       </c>
-      <c r="D10" s="275">
+      <c r="D10" s="276">
         <v>16</v>
       </c>
       <c r="E10" s="92">
@@ -8759,9 +8849,9 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="278"/>
-      <c r="D11" s="276"/>
+    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="279"/>
+      <c r="D11" s="277"/>
       <c r="E11" s="57">
         <v>0</v>
       </c>
@@ -8787,7 +8877,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="143"/>
       <c r="E12" s="143"/>
       <c r="F12" s="143"/>
@@ -8797,7 +8887,7 @@
       <c r="J12" s="143"/>
       <c r="K12" s="143"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="143"/>
       <c r="E13" s="143"/>
       <c r="F13" s="143"/>
@@ -8807,78 +8897,632 @@
       <c r="J13" s="143"/>
       <c r="K13" s="143"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D14" s="143"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="143"/>
-      <c r="I14" s="143"/>
-      <c r="J14" s="143"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="143" t="s">
+        <v>897</v>
+      </c>
+      <c r="E14" s="143" t="s">
+        <v>898</v>
+      </c>
+      <c r="F14" s="143" t="s">
+        <v>899</v>
+      </c>
+      <c r="G14" s="143" t="s">
+        <v>900</v>
+      </c>
+      <c r="H14" t="s">
+        <v>698</v>
+      </c>
+      <c r="I14" t="s">
+        <v>699</v>
+      </c>
+      <c r="J14" t="s">
+        <v>696</v>
+      </c>
       <c r="K14" s="143"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D15" s="143"/>
-      <c r="E15" s="143"/>
-      <c r="F15" s="143"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="143"/>
-      <c r="I15" s="143"/>
-      <c r="J15" s="143"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D15" s="286">
+        <v>16</v>
+      </c>
+      <c r="E15" s="290" t="s">
+        <v>901</v>
+      </c>
+      <c r="F15" s="290" t="s">
+        <v>903</v>
+      </c>
+      <c r="G15" s="290">
+        <v>20</v>
+      </c>
+      <c r="H15" s="290">
+        <f>I15</f>
+        <v>148500000</v>
+      </c>
+      <c r="I15" s="290">
+        <v>148500000</v>
+      </c>
+      <c r="J15" s="290">
+        <f>H15*G15</f>
+        <v>2970000000</v>
+      </c>
       <c r="K15" s="143"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="143"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="143"/>
-      <c r="G16" s="143"/>
-      <c r="H16" s="143"/>
-      <c r="I16" s="143"/>
-      <c r="J16" s="143"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="286"/>
+      <c r="E16" s="290" t="s">
+        <v>902</v>
+      </c>
+      <c r="F16" s="290" t="s">
+        <v>903</v>
+      </c>
+      <c r="G16" s="290">
+        <v>16</v>
+      </c>
+      <c r="H16" s="290">
+        <f>I16</f>
+        <v>148500000</v>
+      </c>
+      <c r="I16" s="290">
+        <v>148500000</v>
+      </c>
+      <c r="J16" s="290">
+        <f>H16*G16</f>
+        <v>2376000000</v>
+      </c>
       <c r="K16" s="143"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D17" s="143"/>
-      <c r="E17" s="143"/>
-      <c r="F17" s="143"/>
-      <c r="G17" s="143"/>
-      <c r="H17" s="143"/>
-      <c r="I17" s="143"/>
-      <c r="J17" s="143"/>
+      <c r="D17" s="285">
+        <v>20</v>
+      </c>
+      <c r="E17" s="290" t="s">
+        <v>902</v>
+      </c>
+      <c r="F17" s="290" t="s">
+        <v>903</v>
+      </c>
+      <c r="G17" s="290">
+        <v>20</v>
+      </c>
+      <c r="H17" s="290">
+        <f>I17</f>
+        <v>148500000</v>
+      </c>
+      <c r="I17" s="290">
+        <v>148500000</v>
+      </c>
+      <c r="J17" s="290">
+        <f>H17*G17</f>
+        <v>2970000000</v>
+      </c>
       <c r="K17" s="143"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
+      <c r="D18" s="286">
+        <v>32</v>
+      </c>
+      <c r="E18" s="290" t="s">
+        <v>901</v>
+      </c>
+      <c r="F18" s="290" t="s">
+        <v>903</v>
+      </c>
+      <c r="G18" s="290">
+        <v>20</v>
+      </c>
+      <c r="H18" s="290">
+        <f>I18*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I18" s="290">
+        <v>148500000</v>
+      </c>
+      <c r="J18" s="290">
+        <f t="shared" ref="J18:J26" si="2">H18*G18</f>
+        <v>5940000000</v>
+      </c>
       <c r="K18" s="143"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D19" s="143"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
+      <c r="D19" s="286"/>
+      <c r="E19" s="291" t="s">
+        <v>902</v>
+      </c>
+      <c r="F19" s="143" t="s">
+        <v>903</v>
+      </c>
+      <c r="G19" s="143">
+        <v>16</v>
+      </c>
+      <c r="H19" s="284">
+        <f>I19*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I19" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J19" s="284">
+        <f t="shared" si="2"/>
+        <v>4752000000</v>
+      </c>
       <c r="K19" s="143"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
+      <c r="D20" s="286"/>
+      <c r="E20" s="291" t="s">
+        <v>901</v>
+      </c>
+      <c r="F20" s="291" t="s">
+        <v>904</v>
+      </c>
+      <c r="G20" s="291">
+        <v>40</v>
+      </c>
+      <c r="H20" s="284">
+        <f>I20</f>
+        <v>148500000</v>
+      </c>
+      <c r="I20" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J20" s="284">
+        <f t="shared" si="2"/>
+        <v>5940000000</v>
+      </c>
       <c r="K20" s="143"/>
     </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D21" s="286"/>
+      <c r="E21" s="291" t="s">
+        <v>902</v>
+      </c>
+      <c r="F21" s="291" t="s">
+        <v>904</v>
+      </c>
+      <c r="G21" s="291">
+        <v>32</v>
+      </c>
+      <c r="H21" s="293">
+        <f>I21</f>
+        <v>148500000</v>
+      </c>
+      <c r="I21" s="294">
+        <v>148500000</v>
+      </c>
+      <c r="J21" s="294">
+        <f t="shared" si="2"/>
+        <v>4752000000</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D22" s="286">
+        <v>40</v>
+      </c>
+      <c r="E22" s="291" t="s">
+        <v>902</v>
+      </c>
+      <c r="F22" s="291" t="s">
+        <v>903</v>
+      </c>
+      <c r="G22" s="291">
+        <v>20</v>
+      </c>
+      <c r="H22" s="287">
+        <f>I22*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I22" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J22" s="284">
+        <f t="shared" si="2"/>
+        <v>5940000000</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="286"/>
+      <c r="E23" s="291" t="s">
+        <v>902</v>
+      </c>
+      <c r="F23" s="291" t="s">
+        <v>904</v>
+      </c>
+      <c r="G23" s="291">
+        <v>40</v>
+      </c>
+      <c r="H23" s="293">
+        <f>I23</f>
+        <v>148500000</v>
+      </c>
+      <c r="I23" s="294">
+        <v>148500000</v>
+      </c>
+      <c r="J23" s="294">
+        <f t="shared" si="2"/>
+        <v>5940000000</v>
+      </c>
+      <c r="K23" s="290"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="286">
+        <v>64</v>
+      </c>
+      <c r="E24" s="222" t="s">
+        <v>901</v>
+      </c>
+      <c r="F24" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G24" s="222">
+        <v>40</v>
+      </c>
+      <c r="H24" s="287">
+        <f>I24*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I24" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J24" s="284">
+        <f t="shared" si="2"/>
+        <v>11880000000</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D25" s="286"/>
+      <c r="E25" s="222" t="s">
+        <v>902</v>
+      </c>
+      <c r="F25" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G25" s="222">
+        <v>32</v>
+      </c>
+      <c r="H25" s="287">
+        <f>I25*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I25" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J25" s="284">
+        <f t="shared" si="2"/>
+        <v>9504000000</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D26" s="289">
+        <v>80</v>
+      </c>
+      <c r="E26" s="222" t="s">
+        <v>902</v>
+      </c>
+      <c r="F26" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G26" s="222">
+        <v>40</v>
+      </c>
+      <c r="H26" s="287">
+        <f>I26*2</f>
+        <v>297000000</v>
+      </c>
+      <c r="I26" s="284">
+        <v>148500000</v>
+      </c>
+      <c r="J26" s="284">
+        <f t="shared" si="2"/>
+        <v>11880000000</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="288"/>
+      <c r="E27" s="222"/>
+      <c r="F27" s="222"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D31" s="222" t="s">
+        <v>897</v>
+      </c>
+      <c r="E31" s="222" t="s">
+        <v>898</v>
+      </c>
+      <c r="F31" s="222" t="s">
+        <v>899</v>
+      </c>
+      <c r="G31" s="222" t="s">
+        <v>900</v>
+      </c>
+      <c r="H31" t="s">
+        <v>698</v>
+      </c>
+      <c r="I31" t="s">
+        <v>699</v>
+      </c>
+      <c r="J31" s="222" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32" s="286">
+        <v>16</v>
+      </c>
+      <c r="E32" s="296" t="s">
+        <v>901</v>
+      </c>
+      <c r="F32" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G32" s="222">
+        <v>20</v>
+      </c>
+      <c r="H32" s="295" t="str">
+        <f>I32</f>
+        <v>148, 5 MHz</v>
+      </c>
+      <c r="I32" s="295" t="s">
+        <v>905</v>
+      </c>
+      <c r="J32" s="295" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D33" s="286"/>
+      <c r="E33" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F33" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G33" s="222">
+        <v>16</v>
+      </c>
+      <c r="H33" s="295" t="str">
+        <f>I33</f>
+        <v>148,5 MHz</v>
+      </c>
+      <c r="I33" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J33" s="295" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D34" s="285">
+        <v>20</v>
+      </c>
+      <c r="E34" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F34" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G34" s="222">
+        <v>20</v>
+      </c>
+      <c r="H34" s="295" t="str">
+        <f>I34</f>
+        <v>148,5 MHz</v>
+      </c>
+      <c r="I34" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J34" s="295" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D35" s="286">
+        <v>32</v>
+      </c>
+      <c r="E35" s="296" t="s">
+        <v>901</v>
+      </c>
+      <c r="F35" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G35" s="222">
+        <v>20</v>
+      </c>
+      <c r="H35" s="295" t="s">
+        <v>909</v>
+      </c>
+      <c r="I35" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J35" s="295" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D36" s="286"/>
+      <c r="E36" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F36" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G36" s="222">
+        <v>16</v>
+      </c>
+      <c r="H36" s="295" t="s">
+        <v>909</v>
+      </c>
+      <c r="I36" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J36" s="295" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D37" s="286"/>
+      <c r="E37" s="296" t="s">
+        <v>901</v>
+      </c>
+      <c r="F37" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G37" s="222">
+        <v>40</v>
+      </c>
+      <c r="H37" s="295" t="str">
+        <f>I37</f>
+        <v>148,5 MHz</v>
+      </c>
+      <c r="I37" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J37" s="295" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D38" s="286"/>
+      <c r="E38" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F38" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G38" s="222">
+        <v>32</v>
+      </c>
+      <c r="H38" s="292" t="s">
+        <v>906</v>
+      </c>
+      <c r="I38" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J38" s="295" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D39" s="286">
+        <v>40</v>
+      </c>
+      <c r="E39" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F39" s="222" t="s">
+        <v>903</v>
+      </c>
+      <c r="G39" s="222">
+        <v>20</v>
+      </c>
+      <c r="H39" s="292" t="s">
+        <v>909</v>
+      </c>
+      <c r="I39" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J39" s="295" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D40" s="286"/>
+      <c r="E40" s="296" t="s">
+        <v>902</v>
+      </c>
+      <c r="F40" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G40" s="222">
+        <v>40</v>
+      </c>
+      <c r="H40" s="287" t="str">
+        <f>I40</f>
+        <v>148,5 MHz</v>
+      </c>
+      <c r="I40" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J40" s="295" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D41" s="286">
+        <v>64</v>
+      </c>
+      <c r="E41" s="222" t="s">
+        <v>901</v>
+      </c>
+      <c r="F41" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G41" s="222">
+        <v>40</v>
+      </c>
+      <c r="H41" s="287" t="s">
+        <v>909</v>
+      </c>
+      <c r="I41" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J41" s="295" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D42" s="286"/>
+      <c r="E42" s="222" t="s">
+        <v>902</v>
+      </c>
+      <c r="F42" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G42" s="222">
+        <v>32</v>
+      </c>
+      <c r="H42" s="287" t="s">
+        <v>909</v>
+      </c>
+      <c r="I42" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J42" s="295" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D43" s="289">
+        <v>80</v>
+      </c>
+      <c r="E43" s="222" t="s">
+        <v>902</v>
+      </c>
+      <c r="F43" s="222" t="s">
+        <v>904</v>
+      </c>
+      <c r="G43" s="222">
+        <v>40</v>
+      </c>
+      <c r="H43" s="287" t="s">
+        <v>909</v>
+      </c>
+      <c r="I43" s="295" t="s">
+        <v>906</v>
+      </c>
+      <c r="J43" s="295" t="s">
+        <v>912</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="15">
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D18:D21"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D6:D7"/>
@@ -8912,59 +9556,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="233" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="232"/>
-      <c r="H1" s="232"/>
-      <c r="I1" s="232"/>
-      <c r="J1" s="232"/>
-      <c r="K1" s="232"/>
-      <c r="L1" s="232"/>
-      <c r="M1" s="232"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="233"/>
+      <c r="H1" s="233"/>
+      <c r="I1" s="233"/>
+      <c r="J1" s="233"/>
+      <c r="K1" s="233"/>
+      <c r="L1" s="233"/>
+      <c r="M1" s="233"/>
     </row>
     <row r="2" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="232"/>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
+      <c r="A2" s="233"/>
+      <c r="B2" s="233"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="233"/>
+      <c r="I2" s="233"/>
+      <c r="J2" s="233"/>
+      <c r="K2" s="233"/>
+      <c r="L2" s="233"/>
+      <c r="M2" s="233"/>
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="232"/>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="T3" s="223" t="s">
+      <c r="A3" s="233"/>
+      <c r="B3" s="233"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="233"/>
+      <c r="L3" s="233"/>
+      <c r="M3" s="233"/>
+      <c r="T3" s="224" t="s">
         <v>196</v>
       </c>
-      <c r="U3" s="224"/>
-      <c r="V3" s="224"/>
-      <c r="W3" s="224"/>
-      <c r="X3" s="224"/>
-      <c r="Y3" s="225"/>
+      <c r="U3" s="225"/>
+      <c r="V3" s="225"/>
+      <c r="W3" s="225"/>
+      <c r="X3" s="225"/>
+      <c r="Y3" s="226"/>
     </row>
     <row r="4" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -9255,14 +9899,14 @@
       <c r="M8" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="233" t="s">
+      <c r="T8" s="234" t="s">
         <v>200</v>
       </c>
-      <c r="U8" s="234"/>
-      <c r="V8" s="234"/>
-      <c r="W8" s="234"/>
-      <c r="X8" s="234"/>
-      <c r="Y8" s="235"/>
+      <c r="U8" s="235"/>
+      <c r="V8" s="235"/>
+      <c r="W8" s="235"/>
+      <c r="X8" s="235"/>
+      <c r="Y8" s="236"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
@@ -10345,22 +10989,22 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="223" t="s">
+      <c r="A39" s="224" t="s">
         <v>404</v>
       </c>
-      <c r="B39" s="224"/>
-      <c r="C39" s="224"/>
-      <c r="D39" s="224"/>
-      <c r="E39" s="224"/>
-      <c r="F39" s="225"/>
-      <c r="H39" s="229" t="s">
+      <c r="B39" s="225"/>
+      <c r="C39" s="225"/>
+      <c r="D39" s="225"/>
+      <c r="E39" s="225"/>
+      <c r="F39" s="226"/>
+      <c r="H39" s="230" t="s">
         <v>403</v>
       </c>
-      <c r="I39" s="230"/>
-      <c r="J39" s="230"/>
-      <c r="K39" s="230"/>
-      <c r="L39" s="230"/>
-      <c r="M39" s="231"/>
+      <c r="I39" s="231"/>
+      <c r="J39" s="231"/>
+      <c r="K39" s="231"/>
+      <c r="L39" s="231"/>
+      <c r="M39" s="232"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10397,52 +11041,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="223" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="242"/>
-      <c r="B2" s="242"/>
-      <c r="C2" s="242"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242"/>
-      <c r="H2" s="242"/>
-      <c r="K2" s="223" t="s">
+      <c r="A2" s="243"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
+      <c r="E2" s="243"/>
+      <c r="F2" s="243"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="243"/>
+      <c r="K2" s="224" t="s">
         <v>332</v>
       </c>
-      <c r="L2" s="224"/>
-      <c r="M2" s="224"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="226"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="246" t="s">
+      <c r="A3" s="247" t="s">
         <v>405</v>
       </c>
-      <c r="B3" s="247"/>
-      <c r="C3" s="247"/>
-      <c r="D3" s="247"/>
-      <c r="E3" s="247"/>
-      <c r="F3" s="247"/>
-      <c r="G3" s="247"/>
-      <c r="H3" s="248"/>
-      <c r="K3" s="243" t="s">
+      <c r="B3" s="248"/>
+      <c r="C3" s="248"/>
+      <c r="D3" s="248"/>
+      <c r="E3" s="248"/>
+      <c r="F3" s="248"/>
+      <c r="G3" s="248"/>
+      <c r="H3" s="249"/>
+      <c r="K3" s="244" t="s">
         <v>312</v>
       </c>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="245"/>
+      <c r="L3" s="245"/>
+      <c r="M3" s="245"/>
+      <c r="N3" s="245"/>
+      <c r="O3" s="246"/>
     </row>
     <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
@@ -10762,13 +11406,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K11" s="236" t="s">
+      <c r="K11" s="237" t="s">
         <v>317</v>
       </c>
-      <c r="L11" s="237"/>
-      <c r="M11" s="237"/>
-      <c r="N11" s="237"/>
-      <c r="O11" s="238"/>
+      <c r="L11" s="238"/>
+      <c r="M11" s="238"/>
+      <c r="N11" s="238"/>
+      <c r="O11" s="239"/>
     </row>
     <row r="12" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
@@ -10796,11 +11440,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K12" s="239"/>
-      <c r="L12" s="240"/>
-      <c r="M12" s="240"/>
-      <c r="N12" s="240"/>
-      <c r="O12" s="241"/>
+      <c r="K12" s="240"/>
+      <c r="L12" s="241"/>
+      <c r="M12" s="241"/>
+      <c r="N12" s="241"/>
+      <c r="O12" s="242"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
@@ -12108,52 +12752,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="223" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="222"/>
-      <c r="C1" s="222"/>
-      <c r="D1" s="222"/>
-      <c r="E1" s="222"/>
-      <c r="F1" s="222"/>
-      <c r="G1" s="222"/>
-      <c r="H1" s="222"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="223"/>
+      <c r="H1" s="223"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="250"/>
-      <c r="B2" s="250"/>
-      <c r="C2" s="250"/>
-      <c r="D2" s="250"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
-      <c r="G2" s="250"/>
-      <c r="H2" s="250"/>
-      <c r="K2" s="223" t="s">
+      <c r="A2" s="251"/>
+      <c r="B2" s="251"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="K2" s="224" t="s">
         <v>425</v>
       </c>
-      <c r="L2" s="224"/>
-      <c r="M2" s="224"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="226"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="254" t="s">
+      <c r="A3" s="255" t="s">
         <v>402</v>
       </c>
-      <c r="B3" s="255"/>
-      <c r="C3" s="255"/>
-      <c r="D3" s="255"/>
-      <c r="E3" s="255"/>
-      <c r="F3" s="255"/>
-      <c r="G3" s="255"/>
-      <c r="H3" s="256"/>
-      <c r="K3" s="251" t="s">
+      <c r="B3" s="256"/>
+      <c r="C3" s="256"/>
+      <c r="D3" s="256"/>
+      <c r="E3" s="256"/>
+      <c r="F3" s="256"/>
+      <c r="G3" s="256"/>
+      <c r="H3" s="257"/>
+      <c r="K3" s="252" t="s">
         <v>426</v>
       </c>
-      <c r="L3" s="252"/>
-      <c r="M3" s="252"/>
-      <c r="N3" s="252"/>
-      <c r="O3" s="253"/>
+      <c r="L3" s="253"/>
+      <c r="M3" s="253"/>
+      <c r="N3" s="253"/>
+      <c r="O3" s="254"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="197" t="s">
@@ -12599,13 +13243,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K14" s="236" t="s">
+      <c r="K14" s="237" t="s">
         <v>317</v>
       </c>
-      <c r="L14" s="237"/>
-      <c r="M14" s="237"/>
-      <c r="N14" s="237"/>
-      <c r="O14" s="238"/>
+      <c r="L14" s="238"/>
+      <c r="M14" s="238"/>
+      <c r="N14" s="238"/>
+      <c r="O14" s="239"/>
     </row>
     <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
@@ -12633,11 +13277,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K15" s="239"/>
-      <c r="L15" s="240"/>
-      <c r="M15" s="240"/>
-      <c r="N15" s="240"/>
-      <c r="O15" s="241"/>
+      <c r="K15" s="240"/>
+      <c r="L15" s="241"/>
+      <c r="M15" s="241"/>
+      <c r="N15" s="241"/>
+      <c r="O15" s="242"/>
     </row>
     <row r="16" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
@@ -13824,16 +14468,16 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="249" t="s">
+      <c r="A55" s="250" t="s">
         <v>417</v>
       </c>
-      <c r="B55" s="249"/>
-      <c r="C55" s="249"/>
-      <c r="D55" s="249"/>
-      <c r="E55" s="249"/>
-      <c r="F55" s="249"/>
-      <c r="G55" s="249"/>
-      <c r="H55" s="249"/>
+      <c r="B55" s="250"/>
+      <c r="C55" s="250"/>
+      <c r="D55" s="250"/>
+      <c r="E55" s="250"/>
+      <c r="F55" s="250"/>
+      <c r="G55" s="250"/>
+      <c r="H55" s="250"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -13879,19 +14523,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="153" t="s">
+        <v>706</v>
+      </c>
+      <c r="B4" s="154" t="s">
+        <v>721</v>
+      </c>
+      <c r="C4" s="154" t="s">
         <v>707</v>
       </c>
-      <c r="B4" s="154" t="s">
-        <v>722</v>
-      </c>
-      <c r="C4" s="154" t="s">
-        <v>708</v>
-      </c>
       <c r="D4" s="154" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E4" s="154" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F4" s="154" t="s">
         <v>0</v>
@@ -13900,40 +14544,40 @@
         <v>688</v>
       </c>
       <c r="H4" s="154" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I4" s="154" t="s">
+        <v>780</v>
+      </c>
+      <c r="J4" s="155" t="s">
         <v>781</v>
-      </c>
-      <c r="J4" s="155" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="174" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B5" s="148">
         <v>1</v>
       </c>
       <c r="C5" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D5" s="102"/>
       <c r="E5" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F5" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G5" s="165" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H5" s="202" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I5" s="202" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="J5" s="203">
         <v>19</v>
@@ -13941,43 +14585,43 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="174" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B6" s="148">
         <v>1</v>
       </c>
       <c r="C6" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D6" s="102"/>
       <c r="E6" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F6" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G6" s="165" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H6" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I6" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J6" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="174" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B7" s="148">
         <v>1</v>
       </c>
       <c r="C7" s="106" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D7" s="106">
         <v>0</v>
@@ -13989,98 +14633,98 @@
         <v>143</v>
       </c>
       <c r="G7" s="166" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H7" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I7" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J7" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L7" s="164"/>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="174" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B8" s="148">
         <v>1</v>
       </c>
       <c r="C8" s="206" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D8" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E8" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F8" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G8" s="166" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H8" s="161" t="s">
+        <v>873</v>
+      </c>
+      <c r="I8" s="161" t="s">
         <v>874</v>
-      </c>
-      <c r="I8" s="161" t="s">
-        <v>875</v>
       </c>
       <c r="J8" s="158">
         <v>114</v>
       </c>
-      <c r="K8" s="260" t="s">
-        <v>839</v>
+      <c r="K8" s="263" t="s">
+        <v>838</v>
       </c>
       <c r="L8" s="164"/>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="174" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B9" s="148">
         <v>1</v>
       </c>
       <c r="C9" s="206" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D9" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E9" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F9" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G9" s="166" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H9" s="161" t="s">
+        <v>875</v>
+      </c>
+      <c r="I9" s="161" t="s">
         <v>876</v>
-      </c>
-      <c r="I9" s="161" t="s">
-        <v>877</v>
       </c>
       <c r="J9" s="158">
         <v>114</v>
       </c>
-      <c r="K9" s="260"/>
+      <c r="K9" s="263"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="181" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B10" s="148">
         <v>1</v>
       </c>
       <c r="C10" s="206"/>
       <c r="D10" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E10" s="102"/>
       <c r="F10" s="148" t="s">
@@ -14088,25 +14732,25 @@
       </c>
       <c r="G10" s="148"/>
       <c r="H10" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I10" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J10" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="181" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B11" s="148">
         <v>1</v>
       </c>
       <c r="C11" s="206"/>
       <c r="D11" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E11" s="102"/>
       <c r="F11" s="148" t="s">
@@ -14114,42 +14758,42 @@
       </c>
       <c r="G11" s="148"/>
       <c r="H11" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I11" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J11" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="174" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B12" s="148">
         <v>1</v>
       </c>
       <c r="C12" s="102" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D12" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E12" s="102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F12" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="148" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H12" s="202" t="s">
+        <v>811</v>
+      </c>
+      <c r="I12" s="202" t="s">
         <v>812</v>
-      </c>
-      <c r="I12" s="202" t="s">
-        <v>813</v>
       </c>
       <c r="J12" s="203">
         <v>19</v>
@@ -14157,31 +14801,31 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="174" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B13" s="148">
         <v>1</v>
       </c>
       <c r="C13" s="102" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D13" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E13" s="102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F13" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="148" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H13" s="202" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I13" s="202" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="J13" s="203">
         <v>19</v>
@@ -14189,327 +14833,327 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="174" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B14" s="148">
         <v>1</v>
       </c>
       <c r="C14" s="206" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D14" s="102">
         <v>0</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F14" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G14" s="148" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H14" s="202" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I14" s="202" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="J14" s="203">
         <v>19</v>
       </c>
-      <c r="K14" s="259" t="s">
-        <v>839</v>
+      <c r="K14" s="262" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="181" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B15" s="148">
         <v>1</v>
       </c>
       <c r="C15" s="102" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D15" s="102" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E15" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F15" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G15" s="148" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H15" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I15" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J15" s="157" t="s">
-        <v>784</v>
-      </c>
-      <c r="K15" s="259"/>
+        <v>783</v>
+      </c>
+      <c r="K15" s="262"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="181" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B16" s="148">
         <v>1</v>
       </c>
       <c r="C16" s="102" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D16" s="198" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E16" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F16" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="148" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H16" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I16" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J16" s="157" t="s">
-        <v>784</v>
-      </c>
-      <c r="K16" s="259"/>
+        <v>783</v>
+      </c>
+      <c r="K16" s="262"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="181" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B17" s="148">
         <v>1</v>
       </c>
       <c r="C17" s="102" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D17" s="102"/>
       <c r="E17" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F17" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="148" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H17" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I17" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J17" s="157" t="s">
-        <v>784</v>
-      </c>
-      <c r="K17" s="259"/>
+        <v>783</v>
+      </c>
+      <c r="K17" s="262"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="181" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B18" s="148">
         <v>1</v>
       </c>
       <c r="C18" s="102" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D18" s="102"/>
       <c r="E18" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F18" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="148" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H18" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I18" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J18" s="157" t="s">
-        <v>784</v>
-      </c>
-      <c r="K18" s="259"/>
+        <v>783</v>
+      </c>
+      <c r="K18" s="262"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="257" t="s">
-        <v>723</v>
-      </c>
-      <c r="B19" s="258"/>
-      <c r="C19" s="258"/>
-      <c r="D19" s="258"/>
-      <c r="E19" s="258"/>
-      <c r="F19" s="258"/>
-      <c r="G19" s="258"/>
+      <c r="A19" s="260" t="s">
+        <v>722</v>
+      </c>
+      <c r="B19" s="261"/>
+      <c r="C19" s="261"/>
+      <c r="D19" s="261"/>
+      <c r="E19" s="261"/>
+      <c r="F19" s="261"/>
+      <c r="G19" s="261"/>
       <c r="H19" s="161"/>
       <c r="I19" s="161"/>
       <c r="J19" s="158"/>
       <c r="K19" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A20" s="174" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B20" s="148">
         <v>9</v>
       </c>
       <c r="C20" s="207" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D20" s="198">
         <v>0</v>
       </c>
       <c r="E20" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F20" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G20" s="185" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H20" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I20" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J20" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="174" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B21" s="148">
         <v>16</v>
       </c>
       <c r="C21" s="207" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D21" s="198">
         <v>0</v>
       </c>
       <c r="E21" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F21" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G21" s="187" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="H21" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I21" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J21" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A22" s="174" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B22" s="148">
         <v>16</v>
       </c>
       <c r="C22" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D22" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E22" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F22" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G22" s="186" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H22" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I22" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J22" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="174" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B23" s="148">
         <v>1</v>
       </c>
       <c r="C23" s="102" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D23" s="102">
         <v>0</v>
       </c>
       <c r="E23" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F23" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G23" s="166" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H23" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I23" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J23" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="174" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B24" s="148">
         <v>1</v>
       </c>
       <c r="C24" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D24" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E24" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F24" s="148" t="s">
         <v>4</v>
@@ -14518,222 +15162,222 @@
         <v>607</v>
       </c>
       <c r="H24" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I24" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J24" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="175" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B25" s="148">
         <v>1</v>
       </c>
       <c r="C25" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D25" s="198">
         <v>0</v>
       </c>
       <c r="E25" s="199" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F25" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G25" s="166" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H25" s="188" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I25" s="189" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J25" s="190" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="265" t="s">
-        <v>730</v>
-      </c>
-      <c r="B26" s="266"/>
-      <c r="C26" s="266"/>
-      <c r="D26" s="266"/>
-      <c r="E26" s="266"/>
-      <c r="F26" s="266"/>
-      <c r="G26" s="266"/>
+      <c r="A26" s="268" t="s">
+        <v>729</v>
+      </c>
+      <c r="B26" s="269"/>
+      <c r="C26" s="269"/>
+      <c r="D26" s="269"/>
+      <c r="E26" s="269"/>
+      <c r="F26" s="269"/>
+      <c r="G26" s="269"/>
       <c r="H26" s="161"/>
       <c r="I26" s="161"/>
       <c r="J26" s="158"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="174" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B27" s="148">
         <v>8</v>
       </c>
       <c r="C27" s="206" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D27" s="102"/>
       <c r="E27" s="106" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F27" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="148" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H27" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I27" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J27" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="261" t="s">
-        <v>732</v>
-      </c>
-      <c r="B28" s="262"/>
-      <c r="C28" s="262"/>
-      <c r="D28" s="262"/>
-      <c r="E28" s="262"/>
-      <c r="F28" s="262"/>
-      <c r="G28" s="262"/>
+      <c r="A28" s="264" t="s">
+        <v>731</v>
+      </c>
+      <c r="B28" s="265"/>
+      <c r="C28" s="265"/>
+      <c r="D28" s="265"/>
+      <c r="E28" s="265"/>
+      <c r="F28" s="265"/>
+      <c r="G28" s="265"/>
       <c r="H28" s="162"/>
       <c r="I28" s="162"/>
       <c r="J28" s="159"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="174" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B29" s="148">
         <v>1</v>
       </c>
       <c r="C29" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D29" s="204">
         <v>0</v>
       </c>
       <c r="E29" s="200" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F29" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G29" s="182" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H29" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I29" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J29" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="174" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B30" s="148">
         <v>1</v>
       </c>
       <c r="C30" s="102" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D30" s="102"/>
       <c r="E30" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F30" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G30" s="166" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H30" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I30" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J30" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="261" t="s">
-        <v>735</v>
-      </c>
-      <c r="B31" s="262"/>
-      <c r="C31" s="262"/>
-      <c r="D31" s="262"/>
-      <c r="E31" s="262"/>
-      <c r="F31" s="262"/>
-      <c r="G31" s="262"/>
+      <c r="A31" s="264" t="s">
+        <v>734</v>
+      </c>
+      <c r="B31" s="265"/>
+      <c r="C31" s="265"/>
+      <c r="D31" s="265"/>
+      <c r="E31" s="265"/>
+      <c r="F31" s="265"/>
+      <c r="G31" s="265"/>
       <c r="H31" s="162"/>
       <c r="I31" s="162"/>
       <c r="J31" s="159"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="174" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B32" s="148">
         <v>1</v>
       </c>
       <c r="C32" s="206" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D32" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E32" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F32" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="148" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H32" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I32" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J32" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="174" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B33" s="148">
         <v>1</v>
       </c>
       <c r="C33" s="198" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D33" s="198">
         <v>0</v>
@@ -14745,101 +15389,101 @@
         <v>143</v>
       </c>
       <c r="G33" s="183" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H33" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I33" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J33" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="261" t="s">
-        <v>738</v>
-      </c>
-      <c r="B34" s="262"/>
-      <c r="C34" s="262"/>
-      <c r="D34" s="262"/>
-      <c r="E34" s="262"/>
-      <c r="F34" s="262"/>
-      <c r="G34" s="262"/>
+      <c r="A34" s="264" t="s">
+        <v>737</v>
+      </c>
+      <c r="B34" s="265"/>
+      <c r="C34" s="265"/>
+      <c r="D34" s="265"/>
+      <c r="E34" s="265"/>
+      <c r="F34" s="265"/>
+      <c r="G34" s="265"/>
       <c r="H34" s="162"/>
       <c r="I34" s="162"/>
       <c r="J34" s="159"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="174" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B35" s="148">
         <v>40</v>
       </c>
       <c r="C35" s="102" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D35" s="102"/>
       <c r="E35" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F35" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G35" s="148" t="s">
+        <v>739</v>
+      </c>
+      <c r="H35" s="156" t="s">
+        <v>783</v>
+      </c>
+      <c r="I35" s="156" t="s">
+        <v>783</v>
+      </c>
+      <c r="J35" s="157" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="264" t="s">
         <v>740</v>
       </c>
-      <c r="H35" s="156" t="s">
-        <v>784</v>
-      </c>
-      <c r="I35" s="156" t="s">
-        <v>784</v>
-      </c>
-      <c r="J35" s="157" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="261" t="s">
-        <v>741</v>
-      </c>
-      <c r="B36" s="262"/>
-      <c r="C36" s="262"/>
-      <c r="D36" s="262"/>
-      <c r="E36" s="262"/>
-      <c r="F36" s="262"/>
-      <c r="G36" s="262"/>
+      <c r="B36" s="265"/>
+      <c r="C36" s="265"/>
+      <c r="D36" s="265"/>
+      <c r="E36" s="265"/>
+      <c r="F36" s="265"/>
+      <c r="G36" s="265"/>
       <c r="H36" s="162"/>
       <c r="I36" s="162"/>
       <c r="J36" s="159"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="174" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B37" s="67">
         <v>1</v>
       </c>
       <c r="C37" s="102" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D37" s="102"/>
       <c r="E37" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F37" s="67" t="s">
         <v>143</v>
       </c>
       <c r="G37" s="67" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H37" s="161" t="s">
+        <v>877</v>
+      </c>
+      <c r="I37" s="161" t="s">
         <v>878</v>
-      </c>
-      <c r="I37" s="161" t="s">
-        <v>879</v>
       </c>
       <c r="J37" s="158">
         <v>114</v>
@@ -14847,413 +15491,413 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="174" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B38" s="148">
         <v>1</v>
       </c>
       <c r="C38" s="102" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D38" s="102"/>
       <c r="E38" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F38" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G38" s="148" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H38" s="161" t="s">
+        <v>879</v>
+      </c>
+      <c r="I38" s="161" t="s">
         <v>880</v>
-      </c>
-      <c r="I38" s="161" t="s">
-        <v>881</v>
       </c>
       <c r="J38" s="158">
         <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="263" t="s">
-        <v>743</v>
-      </c>
-      <c r="B39" s="264"/>
-      <c r="C39" s="264"/>
-      <c r="D39" s="264"/>
-      <c r="E39" s="264"/>
-      <c r="F39" s="264"/>
-      <c r="G39" s="264"/>
+      <c r="A39" s="266" t="s">
+        <v>742</v>
+      </c>
+      <c r="B39" s="267"/>
+      <c r="C39" s="267"/>
+      <c r="D39" s="267"/>
+      <c r="E39" s="267"/>
+      <c r="F39" s="267"/>
+      <c r="G39" s="267"/>
       <c r="H39" s="162"/>
       <c r="I39" s="162"/>
       <c r="J39" s="159"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="174" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B40" s="148">
         <v>1</v>
       </c>
       <c r="C40" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D40" s="204"/>
       <c r="E40" s="200" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F40" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G40" s="148" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H40" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I40" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J40" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="174" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B41" s="148">
         <v>7</v>
       </c>
       <c r="C41" s="206" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D41" s="205" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E41" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F41" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G41" s="148" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H41" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I41" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J41" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="174" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B42" s="148">
         <v>2</v>
       </c>
       <c r="C42" s="102" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D42" s="102">
         <v>0</v>
       </c>
       <c r="E42" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F42" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G42" s="148" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H42" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I42" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J42" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="261" t="s">
-        <v>747</v>
-      </c>
-      <c r="B43" s="262"/>
-      <c r="C43" s="262"/>
-      <c r="D43" s="262"/>
-      <c r="E43" s="262"/>
-      <c r="F43" s="262"/>
-      <c r="G43" s="262"/>
+      <c r="A43" s="264" t="s">
+        <v>746</v>
+      </c>
+      <c r="B43" s="265"/>
+      <c r="C43" s="265"/>
+      <c r="D43" s="265"/>
+      <c r="E43" s="265"/>
+      <c r="F43" s="265"/>
+      <c r="G43" s="265"/>
       <c r="H43" s="162"/>
       <c r="I43" s="162"/>
       <c r="J43" s="159"/>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="174" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B44" s="148">
         <v>1</v>
       </c>
       <c r="C44" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D44" s="102">
         <v>0</v>
       </c>
       <c r="E44" s="102" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F44" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G44" s="166" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H44" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I44" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J44" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="174" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B45" s="148">
         <v>1</v>
       </c>
       <c r="C45" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D45" s="204"/>
       <c r="E45" s="200" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F45" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G45" s="148" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H45" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I45" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J45" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="174" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B46" s="148">
         <v>1</v>
       </c>
       <c r="C46" s="102" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D46" s="102"/>
       <c r="E46" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F46" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G46" s="148" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H46" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I46" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J46" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="257" t="s">
-        <v>751</v>
-      </c>
-      <c r="B47" s="258"/>
-      <c r="C47" s="258"/>
-      <c r="D47" s="258"/>
-      <c r="E47" s="258"/>
-      <c r="F47" s="258"/>
-      <c r="G47" s="258"/>
+      <c r="A47" s="260" t="s">
+        <v>750</v>
+      </c>
+      <c r="B47" s="261"/>
+      <c r="C47" s="261"/>
+      <c r="D47" s="261"/>
+      <c r="E47" s="261"/>
+      <c r="F47" s="261"/>
+      <c r="G47" s="261"/>
       <c r="H47" s="163"/>
       <c r="I47" s="163"/>
       <c r="J47" s="160"/>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="174" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B48" s="148">
         <v>1</v>
       </c>
       <c r="C48" s="102" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D48" s="204">
         <v>0</v>
       </c>
       <c r="E48" s="200" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F48" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G48" s="166" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H48" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I48" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J48" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="174" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B49" s="148">
         <v>1</v>
       </c>
       <c r="C49" s="102" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D49" s="102">
         <v>0</v>
       </c>
       <c r="E49" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F49" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G49" s="166" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H49" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I49" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J49" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="267" t="s">
-        <v>755</v>
-      </c>
-      <c r="B50" s="268"/>
-      <c r="C50" s="268"/>
-      <c r="D50" s="268"/>
-      <c r="E50" s="268"/>
-      <c r="F50" s="268"/>
-      <c r="G50" s="268"/>
+      <c r="A50" s="258" t="s">
+        <v>754</v>
+      </c>
+      <c r="B50" s="259"/>
+      <c r="C50" s="259"/>
+      <c r="D50" s="259"/>
+      <c r="E50" s="259"/>
+      <c r="F50" s="259"/>
+      <c r="G50" s="259"/>
       <c r="H50" s="163"/>
       <c r="I50" s="163"/>
       <c r="J50" s="160"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="175" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B51" s="148">
         <v>40</v>
       </c>
       <c r="C51" s="102" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D51" s="102" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E51" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F51" s="148" t="s">
         <v>143</v>
       </c>
       <c r="G51" s="148" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H51" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I51" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J51" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="267" t="s">
-        <v>756</v>
-      </c>
-      <c r="B52" s="268"/>
-      <c r="C52" s="268"/>
-      <c r="D52" s="268"/>
-      <c r="E52" s="268"/>
-      <c r="F52" s="268"/>
-      <c r="G52" s="268"/>
+      <c r="A52" s="258" t="s">
+        <v>755</v>
+      </c>
+      <c r="B52" s="259"/>
+      <c r="C52" s="259"/>
+      <c r="D52" s="259"/>
+      <c r="E52" s="259"/>
+      <c r="F52" s="259"/>
+      <c r="G52" s="259"/>
       <c r="H52" s="163"/>
       <c r="I52" s="163"/>
       <c r="J52" s="160"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="174" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B53" s="148">
         <v>1</v>
       </c>
       <c r="C53" s="102" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D53" s="102" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E53" s="102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F53" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G53" s="148" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H53" s="161" t="s">
+        <v>881</v>
+      </c>
+      <c r="I53" s="161" t="s">
         <v>882</v>
-      </c>
-      <c r="I53" s="161" t="s">
-        <v>883</v>
       </c>
       <c r="J53" s="158">
         <v>114</v>
@@ -15261,65 +15905,65 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="174" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B54" s="148">
         <v>1</v>
       </c>
       <c r="C54" s="102" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D54" s="102" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E54" s="102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F54" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G54" s="148" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H54" s="161" t="s">
+        <v>883</v>
+      </c>
+      <c r="I54" s="161" t="s">
         <v>884</v>
-      </c>
-      <c r="I54" s="161" t="s">
-        <v>885</v>
       </c>
       <c r="J54" s="158">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="267" t="s">
-        <v>760</v>
-      </c>
-      <c r="B55" s="268"/>
-      <c r="C55" s="268"/>
-      <c r="D55" s="268"/>
-      <c r="E55" s="268"/>
-      <c r="F55" s="268"/>
-      <c r="G55" s="268"/>
+      <c r="A55" s="258" t="s">
+        <v>759</v>
+      </c>
+      <c r="B55" s="259"/>
+      <c r="C55" s="259"/>
+      <c r="D55" s="259"/>
+      <c r="E55" s="259"/>
+      <c r="F55" s="259"/>
+      <c r="G55" s="259"/>
       <c r="H55" s="163"/>
       <c r="I55" s="163"/>
       <c r="J55" s="160"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="181" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B56" s="148">
         <v>1</v>
       </c>
       <c r="C56" s="102" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D56" s="205" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E56" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F56" s="148" t="s">
         <v>4</v>
@@ -15331,19 +15975,19 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="181" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B57" s="148">
         <v>1</v>
       </c>
       <c r="C57" s="102" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D57" s="205" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E57" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F57" s="148" t="s">
         <v>4</v>
@@ -15354,74 +15998,74 @@
       <c r="J57" s="49"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="267" t="s">
-        <v>763</v>
-      </c>
-      <c r="B58" s="268"/>
-      <c r="C58" s="268"/>
-      <c r="D58" s="268"/>
-      <c r="E58" s="268"/>
-      <c r="F58" s="268"/>
-      <c r="G58" s="268"/>
+      <c r="A58" s="258" t="s">
+        <v>762</v>
+      </c>
+      <c r="B58" s="259"/>
+      <c r="C58" s="259"/>
+      <c r="D58" s="259"/>
+      <c r="E58" s="259"/>
+      <c r="F58" s="259"/>
+      <c r="G58" s="259"/>
       <c r="H58" s="163"/>
       <c r="I58" s="163"/>
       <c r="J58" s="160"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="174" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B59" s="148">
         <v>1</v>
       </c>
       <c r="C59" s="102" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D59" s="102" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E59" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F59" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G59" s="148" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H59" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I59" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J59" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="257" t="s">
-        <v>765</v>
-      </c>
-      <c r="B60" s="258"/>
-      <c r="C60" s="258"/>
-      <c r="D60" s="258"/>
-      <c r="E60" s="258"/>
-      <c r="F60" s="258"/>
-      <c r="G60" s="258"/>
+      <c r="A60" s="260" t="s">
+        <v>764</v>
+      </c>
+      <c r="B60" s="261"/>
+      <c r="C60" s="261"/>
+      <c r="D60" s="261"/>
+      <c r="E60" s="261"/>
+      <c r="F60" s="261"/>
+      <c r="G60" s="261"/>
       <c r="H60" s="161"/>
       <c r="I60" s="161"/>
       <c r="J60" s="158"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="191" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B61" s="192">
         <v>8</v>
       </c>
       <c r="C61" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D61" s="193"/>
       <c r="E61" s="193"/>
@@ -15429,27 +16073,27 @@
         <v>143</v>
       </c>
       <c r="G61" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H61" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I61" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J61" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="191" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B62" s="192">
         <v>16</v>
       </c>
       <c r="C62" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D62" s="193"/>
       <c r="E62" s="193"/>
@@ -15457,27 +16101,27 @@
         <v>143</v>
       </c>
       <c r="G62" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H62" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I62" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J62" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="191" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B63" s="192">
         <v>16</v>
       </c>
       <c r="C63" s="196" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D63" s="196"/>
       <c r="E63" s="196"/>
@@ -15485,27 +16129,27 @@
         <v>143</v>
       </c>
       <c r="G63" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H63" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I63" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J63" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="191" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B64" s="192">
         <v>1</v>
       </c>
       <c r="C64" s="192" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D64" s="192"/>
       <c r="E64" s="192"/>
@@ -15513,27 +16157,27 @@
         <v>143</v>
       </c>
       <c r="G64" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H64" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I64" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J64" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="191" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B65" s="192">
         <v>1</v>
       </c>
       <c r="C65" s="196" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D65" s="196"/>
       <c r="E65" s="196"/>
@@ -15541,27 +16185,27 @@
         <v>4</v>
       </c>
       <c r="G65" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H65" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I65" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J65" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="191" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B66" s="192">
         <v>1</v>
       </c>
       <c r="C66" s="196" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D66" s="196"/>
       <c r="E66" s="196"/>
@@ -15569,183 +16213,183 @@
         <v>143</v>
       </c>
       <c r="G66" s="193" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H66" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I66" s="194" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J66" s="195" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="257" t="s">
-        <v>772</v>
-      </c>
-      <c r="B67" s="258"/>
-      <c r="C67" s="258"/>
-      <c r="D67" s="258"/>
-      <c r="E67" s="258"/>
-      <c r="F67" s="258"/>
-      <c r="G67" s="258"/>
+      <c r="A67" s="260" t="s">
+        <v>771</v>
+      </c>
+      <c r="B67" s="261"/>
+      <c r="C67" s="261"/>
+      <c r="D67" s="261"/>
+      <c r="E67" s="261"/>
+      <c r="F67" s="261"/>
+      <c r="G67" s="261"/>
       <c r="H67" s="161"/>
       <c r="I67" s="161"/>
       <c r="J67" s="158"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="181" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B68" s="148">
         <v>1</v>
       </c>
       <c r="C68" s="102" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D68" s="102"/>
       <c r="E68" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F68" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G68" s="148" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H68" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I68" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J68" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="181" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B69" s="148">
         <v>1</v>
       </c>
       <c r="C69" s="102" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D69" s="102"/>
       <c r="E69" s="102" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F69" s="148" t="s">
         <v>4</v>
       </c>
       <c r="G69" s="117" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H69" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I69" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J69" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="184" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B70" s="152">
         <v>1</v>
       </c>
       <c r="C70" s="140" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D70" s="140"/>
       <c r="E70" s="140" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F70" s="152" t="s">
         <v>4</v>
       </c>
       <c r="G70" s="117" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H70" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I70" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J70" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="184" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B71" s="152">
         <v>1</v>
       </c>
       <c r="C71" s="140" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D71" s="140"/>
       <c r="E71" s="140" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F71" s="152" t="s">
         <v>4</v>
       </c>
       <c r="G71" s="117" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H71" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I71" s="156" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J71" s="157" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="180" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B72" s="149">
         <v>1</v>
       </c>
       <c r="C72" s="107" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D72" s="107"/>
       <c r="E72" s="107" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F72" s="149" t="s">
         <v>4</v>
       </c>
       <c r="G72" s="179" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H72" s="177" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I72" s="177" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J72" s="178" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K72" s="201" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -15761,19 +16405,19 @@
       <c r="A74" s="151"/>
       <c r="B74" s="151"/>
       <c r="C74" s="151" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D74" s="151"/>
       <c r="E74" s="151" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F74" s="151"/>
       <c r="G74" s="151"/>
       <c r="H74" s="143" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I74" s="143" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="J74" s="143">
         <v>19</v>
@@ -15817,6 +16461,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A55:G55"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="K14:K18"/>
@@ -15833,7 +16478,6 @@
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A55:G55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15861,7 +16505,7 @@
       <c r="B1" s="210"/>
       <c r="C1" s="210"/>
       <c r="D1" s="168" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E1" s="210" t="s">
         <v>3</v>
@@ -15872,7 +16516,7 @@
       <c r="G1" s="216"/>
       <c r="H1" s="210"/>
       <c r="I1" s="168" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="J1" s="210" t="s">
         <v>3</v>
@@ -17182,7 +17826,7 @@
         <v>533</v>
       </c>
       <c r="I41" s="173" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="J41" s="109" t="s">
         <v>148</v>
@@ -17311,17 +17955,17 @@
       <c r="K50" s="58"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="254" t="s">
+      <c r="A54" s="255" t="s">
         <v>402</v>
       </c>
-      <c r="B54" s="255"/>
-      <c r="C54" s="255"/>
-      <c r="D54" s="255"/>
-      <c r="E54" s="255"/>
-      <c r="F54" s="255"/>
-      <c r="G54" s="255"/>
-      <c r="H54" s="255"/>
-      <c r="I54" s="256"/>
+      <c r="B54" s="256"/>
+      <c r="C54" s="256"/>
+      <c r="D54" s="256"/>
+      <c r="E54" s="256"/>
+      <c r="F54" s="256"/>
+      <c r="G54" s="256"/>
+      <c r="H54" s="256"/>
+      <c r="I54" s="257"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="197" t="s">
@@ -17358,7 +18002,7 @@
         <v>550</v>
       </c>
       <c r="C56" s="173" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D56" s="173" t="s">
         <v>42</v>
@@ -17387,7 +18031,7 @@
         <v>551</v>
       </c>
       <c r="C57" s="173" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D57" s="173" t="s">
         <v>41</v>
@@ -17417,7 +18061,7 @@
         <v>552</v>
       </c>
       <c r="C58" s="173" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D58" s="173" t="s">
         <v>44</v>
@@ -17447,7 +18091,7 @@
         <v>553</v>
       </c>
       <c r="C59" s="173" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D59" s="173" t="s">
         <v>43</v>
@@ -18602,28 +19246,28 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="221" t="s">
+        <v>893</v>
+      </c>
+      <c r="B5" s="221" t="s">
         <v>894</v>
-      </c>
-      <c r="B5" s="221" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="221" t="s">
+        <v>895</v>
+      </c>
+      <c r="B6" s="221" t="s">
         <v>896</v>
-      </c>
-      <c r="B6" s="221" t="s">
-        <v>897</v>
       </c>
     </row>
   </sheetData>
@@ -18648,11 +19292,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="269" t="s">
+      <c r="A2" s="270" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="270"/>
-      <c r="C2" s="271"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="272"/>
     </row>
     <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -18754,19 +19398,19 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="269" t="s">
+      <c r="A12" s="270" t="s">
         <v>359</v>
       </c>
-      <c r="B12" s="270"/>
-      <c r="C12" s="271"/>
+      <c r="B12" s="271"/>
+      <c r="C12" s="272"/>
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="269" t="s">
+      <c r="A15" s="270" t="s">
         <v>361</v>
       </c>
-      <c r="B15" s="270"/>
-      <c r="C15" s="271"/>
+      <c r="B15" s="271"/>
+      <c r="C15" s="272"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
@@ -18868,19 +19512,19 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="269" t="s">
+      <c r="A25" s="270" t="s">
         <v>359</v>
       </c>
-      <c r="B25" s="270"/>
-      <c r="C25" s="271"/>
+      <c r="B25" s="271"/>
+      <c r="C25" s="272"/>
     </row>
     <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="269" t="s">
+      <c r="A28" s="270" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="270"/>
-      <c r="C28" s="271"/>
+      <c r="B28" s="271"/>
+      <c r="C28" s="272"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
@@ -18980,11 +19624,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="269" t="s">
+      <c r="A38" s="270" t="s">
         <v>359</v>
       </c>
-      <c r="B38" s="270"/>
-      <c r="C38" s="271"/>
+      <c r="B38" s="271"/>
+      <c r="C38" s="272"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -21542,7 +22186,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="272" t="s">
+      <c r="G107" s="273" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -21578,7 +22222,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="273"/>
+      <c r="G108" s="274"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -21616,7 +22260,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="274" t="s">
+      <c r="J109" s="275" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -21638,7 +22282,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="274"/>
+      <c r="J110" s="275"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -21658,7 +22302,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="274"/>
+      <c r="J111" s="275"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -21678,7 +22322,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="274"/>
+      <c r="J112" s="275"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
21 de junho - INESC
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/Book1.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoA" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="ReferenceDesign_1channel+audio" sheetId="6" r:id="rId9"/>
     <sheet name="ReferenceDesign_1channel+au (2)" sheetId="7" r:id="rId10"/>
     <sheet name="Line Rates Calculation" sheetId="8" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="933">
   <si>
     <t>I/O</t>
   </si>
@@ -2785,6 +2786,60 @@
   </si>
   <si>
     <t>Velocidade em série</t>
+  </si>
+  <si>
+    <t>TX Line Rate (Gb/s)</t>
+  </si>
+  <si>
+    <t>TX Reference Clock (MHz)</t>
+  </si>
+  <si>
+    <t>Enconding</t>
+  </si>
+  <si>
+    <t>TX Internal Data Width</t>
+  </si>
+  <si>
+    <t>TX External Data Width</t>
+  </si>
+  <si>
+    <t>TXUSRCLK (MHz)</t>
+  </si>
+  <si>
+    <t>TXUSRCLK2 (MHz)</t>
+  </si>
+  <si>
+    <t>TX Buffer Enabled</t>
+  </si>
+  <si>
+    <t>RX Line Rate (Gb/s)</t>
+  </si>
+  <si>
+    <t>RX Reference Clock (MHz)</t>
+  </si>
+  <si>
+    <t>Decoding</t>
+  </si>
+  <si>
+    <t>RX Internal Data Width</t>
+  </si>
+  <si>
+    <t>RX External Data Width</t>
+  </si>
+  <si>
+    <t>RXUSRCLK (MHz)</t>
+  </si>
+  <si>
+    <t>RXUSRCLK2 (MHz)</t>
+  </si>
+  <si>
+    <t>RX Buffer Enabled</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Plano D</t>
   </si>
 </sst>
 </file>
@@ -2792,7 +2847,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -3816,7 +3871,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="297">
+  <cellXfs count="298">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -4428,199 +4483,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4629,18 +4498,207 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -4967,60 +5025,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="235" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
-      <c r="I1" s="223"/>
-      <c r="J1" s="223"/>
-      <c r="K1" s="223"/>
-      <c r="L1" s="223"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="223"/>
-      <c r="O1" s="223"/>
-      <c r="P1" s="223"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
+      <c r="N1" s="235"/>
+      <c r="O1" s="235"/>
+      <c r="P1" s="235"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="223"/>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="223"/>
-      <c r="L2" s="223"/>
-      <c r="M2" s="223"/>
-      <c r="N2" s="223"/>
-      <c r="O2" s="223"/>
-      <c r="P2" s="223"/>
+      <c r="A2" s="235"/>
+      <c r="B2" s="235"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
+      <c r="I2" s="235"/>
+      <c r="J2" s="235"/>
+      <c r="K2" s="235"/>
+      <c r="L2" s="235"/>
+      <c r="M2" s="235"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
+      <c r="P2" s="235"/>
     </row>
     <row r="3" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="223"/>
-      <c r="B3" s="223"/>
-      <c r="C3" s="223"/>
-      <c r="D3" s="223"/>
-      <c r="E3" s="223"/>
-      <c r="F3" s="223"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="223"/>
-      <c r="I3" s="223"/>
-      <c r="J3" s="223"/>
-      <c r="K3" s="223"/>
-      <c r="L3" s="223"/>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="223"/>
+      <c r="A3" s="235"/>
+      <c r="B3" s="235"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="235"/>
+      <c r="I3" s="235"/>
+      <c r="J3" s="235"/>
+      <c r="K3" s="235"/>
+      <c r="L3" s="235"/>
+      <c r="M3" s="235"/>
+      <c r="N3" s="235"/>
+      <c r="O3" s="235"/>
+      <c r="P3" s="235"/>
     </row>
     <row r="4" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -5053,14 +5111,14 @@
       <c r="K4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="224" t="s">
+      <c r="M4" s="236" t="s">
         <v>196</v>
       </c>
-      <c r="N4" s="225"/>
-      <c r="O4" s="225"/>
-      <c r="P4" s="225"/>
-      <c r="Q4" s="225"/>
-      <c r="R4" s="226"/>
+      <c r="N4" s="237"/>
+      <c r="O4" s="237"/>
+      <c r="P4" s="237"/>
+      <c r="Q4" s="237"/>
+      <c r="R4" s="238"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -5281,14 +5339,14 @@
       <c r="F9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="227" t="s">
+      <c r="M9" s="239" t="s">
         <v>200</v>
       </c>
-      <c r="N9" s="228"/>
-      <c r="O9" s="228"/>
-      <c r="P9" s="228"/>
-      <c r="Q9" s="228"/>
-      <c r="R9" s="229"/>
+      <c r="N9" s="240"/>
+      <c r="O9" s="240"/>
+      <c r="P9" s="240"/>
+      <c r="Q9" s="240"/>
+      <c r="R9" s="241"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -5871,14 +5929,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="230" t="s">
+      <c r="A39" s="242" t="s">
         <v>403</v>
       </c>
-      <c r="B39" s="231"/>
-      <c r="C39" s="231"/>
-      <c r="D39" s="231"/>
-      <c r="E39" s="231"/>
-      <c r="F39" s="232"/>
+      <c r="B39" s="243"/>
+      <c r="C39" s="243"/>
+      <c r="D39" s="243"/>
+      <c r="E39" s="243"/>
+      <c r="F39" s="244"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8435,7 +8493,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="273" t="s">
+      <c r="G107" s="285" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -8471,7 +8529,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="274"/>
+      <c r="G108" s="286"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -8509,7 +8567,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="275" t="s">
+      <c r="J109" s="287" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -8537,7 +8595,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="275"/>
+      <c r="J110" s="287"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -8557,7 +8615,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="275"/>
+      <c r="J111" s="287"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -8577,7 +8635,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="275"/>
+      <c r="J112" s="287"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>
@@ -8641,7 +8699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScale="150" workbookViewId="0">
       <selection activeCell="B39" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
@@ -8700,10 +8758,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="282" t="s">
+      <c r="C6" s="295" t="s">
         <v>703</v>
       </c>
-      <c r="D6" s="280">
+      <c r="D6" s="293">
         <v>64</v>
       </c>
       <c r="E6" s="46">
@@ -8732,8 +8790,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C7" s="283"/>
-      <c r="D7" s="276"/>
+      <c r="C7" s="296"/>
+      <c r="D7" s="289"/>
       <c r="E7" s="92">
         <v>1</v>
       </c>
@@ -8760,13 +8818,13 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="278" t="s">
+      <c r="C8" s="291" t="s">
         <v>704</v>
       </c>
-      <c r="D8" s="281">
+      <c r="D8" s="294">
         <v>40</v>
       </c>
-      <c r="E8" s="281">
+      <c r="E8" s="294">
         <v>0</v>
       </c>
       <c r="F8" s="67">
@@ -8792,9 +8850,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="278"/>
-      <c r="D9" s="281"/>
-      <c r="E9" s="281"/>
+      <c r="C9" s="291"/>
+      <c r="D9" s="294"/>
+      <c r="E9" s="294"/>
       <c r="F9" s="92">
         <v>1</v>
       </c>
@@ -8818,10 +8876,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="278" t="s">
+      <c r="C10" s="291" t="s">
         <v>705</v>
       </c>
-      <c r="D10" s="276">
+      <c r="D10" s="289">
         <v>16</v>
       </c>
       <c r="E10" s="92">
@@ -8850,8 +8908,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="279"/>
-      <c r="D11" s="277"/>
+      <c r="C11" s="292"/>
+      <c r="D11" s="290"/>
       <c r="E11" s="57">
         <v>0</v>
       </c>
@@ -8922,110 +8980,110 @@
       <c r="K14" s="143"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="286">
+      <c r="D15" s="288">
         <v>16</v>
       </c>
-      <c r="E15" s="290" t="s">
+      <c r="E15" s="228" t="s">
         <v>901</v>
       </c>
-      <c r="F15" s="290" t="s">
+      <c r="F15" s="228" t="s">
         <v>903</v>
       </c>
-      <c r="G15" s="290">
+      <c r="G15" s="228">
         <v>20</v>
       </c>
-      <c r="H15" s="290">
+      <c r="H15" s="228">
         <f>I15</f>
         <v>148500000</v>
       </c>
-      <c r="I15" s="290">
+      <c r="I15" s="228">
         <v>148500000</v>
       </c>
-      <c r="J15" s="290">
+      <c r="J15" s="228">
         <f>H15*G15</f>
         <v>2970000000</v>
       </c>
       <c r="K15" s="143"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="286"/>
-      <c r="E16" s="290" t="s">
+      <c r="D16" s="288"/>
+      <c r="E16" s="228" t="s">
         <v>902</v>
       </c>
-      <c r="F16" s="290" t="s">
+      <c r="F16" s="228" t="s">
         <v>903</v>
       </c>
-      <c r="G16" s="290">
+      <c r="G16" s="228">
         <v>16</v>
       </c>
-      <c r="H16" s="290">
+      <c r="H16" s="228">
         <f>I16</f>
         <v>148500000</v>
       </c>
-      <c r="I16" s="290">
+      <c r="I16" s="228">
         <v>148500000</v>
       </c>
-      <c r="J16" s="290">
+      <c r="J16" s="228">
         <f>H16*G16</f>
         <v>2376000000</v>
       </c>
       <c r="K16" s="143"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D17" s="285">
+      <c r="D17" s="224">
         <v>20</v>
       </c>
-      <c r="E17" s="290" t="s">
+      <c r="E17" s="228" t="s">
         <v>902</v>
       </c>
-      <c r="F17" s="290" t="s">
+      <c r="F17" s="228" t="s">
         <v>903</v>
       </c>
-      <c r="G17" s="290">
+      <c r="G17" s="228">
         <v>20</v>
       </c>
-      <c r="H17" s="290">
+      <c r="H17" s="228">
         <f>I17</f>
         <v>148500000</v>
       </c>
-      <c r="I17" s="290">
+      <c r="I17" s="228">
         <v>148500000</v>
       </c>
-      <c r="J17" s="290">
+      <c r="J17" s="228">
         <f>H17*G17</f>
         <v>2970000000</v>
       </c>
       <c r="K17" s="143"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D18" s="286">
+      <c r="D18" s="288">
         <v>32</v>
       </c>
-      <c r="E18" s="290" t="s">
+      <c r="E18" s="228" t="s">
         <v>901</v>
       </c>
-      <c r="F18" s="290" t="s">
+      <c r="F18" s="228" t="s">
         <v>903</v>
       </c>
-      <c r="G18" s="290">
+      <c r="G18" s="228">
         <v>20</v>
       </c>
-      <c r="H18" s="290">
+      <c r="H18" s="228">
         <f>I18*2</f>
         <v>297000000</v>
       </c>
-      <c r="I18" s="290">
+      <c r="I18" s="228">
         <v>148500000</v>
       </c>
-      <c r="J18" s="290">
+      <c r="J18" s="228">
         <f t="shared" ref="J18:J26" si="2">H18*G18</f>
         <v>5940000000</v>
       </c>
       <c r="K18" s="143"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D19" s="286"/>
-      <c r="E19" s="291" t="s">
+      <c r="D19" s="288"/>
+      <c r="E19" s="229" t="s">
         <v>902</v>
       </c>
       <c r="F19" s="143" t="s">
@@ -9034,117 +9092,117 @@
       <c r="G19" s="143">
         <v>16</v>
       </c>
-      <c r="H19" s="284">
+      <c r="H19" s="223">
         <f>I19*2</f>
         <v>297000000</v>
       </c>
-      <c r="I19" s="284">
+      <c r="I19" s="223">
         <v>148500000</v>
       </c>
-      <c r="J19" s="284">
+      <c r="J19" s="223">
         <f t="shared" si="2"/>
         <v>4752000000</v>
       </c>
       <c r="K19" s="143"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="286"/>
-      <c r="E20" s="291" t="s">
+      <c r="D20" s="288"/>
+      <c r="E20" s="229" t="s">
         <v>901</v>
       </c>
-      <c r="F20" s="291" t="s">
+      <c r="F20" s="229" t="s">
         <v>904</v>
       </c>
-      <c r="G20" s="291">
+      <c r="G20" s="229">
         <v>40</v>
       </c>
-      <c r="H20" s="284">
+      <c r="H20" s="223">
         <f>I20</f>
         <v>148500000</v>
       </c>
-      <c r="I20" s="284">
+      <c r="I20" s="223">
         <v>148500000</v>
       </c>
-      <c r="J20" s="284">
+      <c r="J20" s="223">
         <f t="shared" si="2"/>
         <v>5940000000</v>
       </c>
       <c r="K20" s="143"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D21" s="286"/>
-      <c r="E21" s="291" t="s">
+      <c r="D21" s="288"/>
+      <c r="E21" s="229" t="s">
         <v>902</v>
       </c>
-      <c r="F21" s="291" t="s">
+      <c r="F21" s="229" t="s">
         <v>904</v>
       </c>
-      <c r="G21" s="291">
+      <c r="G21" s="229">
         <v>32</v>
       </c>
-      <c r="H21" s="293">
+      <c r="H21" s="231">
         <f>I21</f>
         <v>148500000</v>
       </c>
-      <c r="I21" s="294">
+      <c r="I21" s="232">
         <v>148500000</v>
       </c>
-      <c r="J21" s="294">
+      <c r="J21" s="232">
         <f t="shared" si="2"/>
         <v>4752000000</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="286">
+      <c r="D22" s="288">
         <v>40</v>
       </c>
-      <c r="E22" s="291" t="s">
+      <c r="E22" s="229" t="s">
         <v>902</v>
       </c>
-      <c r="F22" s="291" t="s">
+      <c r="F22" s="229" t="s">
         <v>903</v>
       </c>
-      <c r="G22" s="291">
+      <c r="G22" s="229">
         <v>20</v>
       </c>
-      <c r="H22" s="287">
+      <c r="H22" s="225">
         <f>I22*2</f>
         <v>297000000</v>
       </c>
-      <c r="I22" s="284">
+      <c r="I22" s="223">
         <v>148500000</v>
       </c>
-      <c r="J22" s="284">
+      <c r="J22" s="223">
         <f t="shared" si="2"/>
         <v>5940000000</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D23" s="286"/>
-      <c r="E23" s="291" t="s">
+      <c r="D23" s="288"/>
+      <c r="E23" s="229" t="s">
         <v>902</v>
       </c>
-      <c r="F23" s="291" t="s">
+      <c r="F23" s="229" t="s">
         <v>904</v>
       </c>
-      <c r="G23" s="291">
+      <c r="G23" s="229">
         <v>40</v>
       </c>
-      <c r="H23" s="293">
+      <c r="H23" s="231">
         <f>I23</f>
         <v>148500000</v>
       </c>
-      <c r="I23" s="294">
+      <c r="I23" s="232">
         <v>148500000</v>
       </c>
-      <c r="J23" s="294">
+      <c r="J23" s="232">
         <f t="shared" si="2"/>
         <v>5940000000</v>
       </c>
-      <c r="K23" s="290"/>
+      <c r="K23" s="228"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D24" s="286">
+      <c r="D24" s="288">
         <v>64</v>
       </c>
       <c r="E24" s="222" t="s">
@@ -9156,20 +9214,20 @@
       <c r="G24" s="222">
         <v>40</v>
       </c>
-      <c r="H24" s="287">
+      <c r="H24" s="225">
         <f>I24*2</f>
         <v>297000000</v>
       </c>
-      <c r="I24" s="284">
+      <c r="I24" s="223">
         <v>148500000</v>
       </c>
-      <c r="J24" s="284">
+      <c r="J24" s="223">
         <f t="shared" si="2"/>
         <v>11880000000</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="286"/>
+      <c r="D25" s="288"/>
       <c r="E25" s="222" t="s">
         <v>902</v>
       </c>
@@ -9179,20 +9237,20 @@
       <c r="G25" s="222">
         <v>32</v>
       </c>
-      <c r="H25" s="287">
+      <c r="H25" s="225">
         <f>I25*2</f>
         <v>297000000</v>
       </c>
-      <c r="I25" s="284">
+      <c r="I25" s="223">
         <v>148500000</v>
       </c>
-      <c r="J25" s="284">
+      <c r="J25" s="223">
         <f t="shared" si="2"/>
         <v>9504000000</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D26" s="289">
+      <c r="D26" s="227">
         <v>80</v>
       </c>
       <c r="E26" s="222" t="s">
@@ -9204,20 +9262,20 @@
       <c r="G26" s="222">
         <v>40</v>
       </c>
-      <c r="H26" s="287">
+      <c r="H26" s="225">
         <f>I26*2</f>
         <v>297000000</v>
       </c>
-      <c r="I26" s="284">
+      <c r="I26" s="223">
         <v>148500000</v>
       </c>
-      <c r="J26" s="284">
+      <c r="J26" s="223">
         <f t="shared" si="2"/>
         <v>11880000000</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D27" s="288"/>
+      <c r="D27" s="226"/>
       <c r="E27" s="222"/>
       <c r="F27" s="222"/>
     </row>
@@ -9245,10 +9303,10 @@
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D32" s="286">
+      <c r="D32" s="288">
         <v>16</v>
       </c>
-      <c r="E32" s="296" t="s">
+      <c r="E32" s="234" t="s">
         <v>901</v>
       </c>
       <c r="F32" s="222" t="s">
@@ -9257,20 +9315,20 @@
       <c r="G32" s="222">
         <v>20</v>
       </c>
-      <c r="H32" s="295" t="str">
+      <c r="H32" s="233" t="str">
         <f>I32</f>
         <v>148, 5 MHz</v>
       </c>
-      <c r="I32" s="295" t="s">
+      <c r="I32" s="233" t="s">
         <v>905</v>
       </c>
-      <c r="J32" s="295" t="s">
+      <c r="J32" s="233" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D33" s="286"/>
-      <c r="E33" s="296" t="s">
+      <c r="D33" s="288"/>
+      <c r="E33" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F33" s="222" t="s">
@@ -9279,22 +9337,22 @@
       <c r="G33" s="222">
         <v>16</v>
       </c>
-      <c r="H33" s="295" t="str">
+      <c r="H33" s="233" t="str">
         <f>I33</f>
         <v>148,5 MHz</v>
       </c>
-      <c r="I33" s="295" t="s">
+      <c r="I33" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J33" s="295" t="s">
+      <c r="J33" s="233" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D34" s="285">
+      <c r="D34" s="224">
         <v>20</v>
       </c>
-      <c r="E34" s="296" t="s">
+      <c r="E34" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F34" s="222" t="s">
@@ -9303,22 +9361,22 @@
       <c r="G34" s="222">
         <v>20</v>
       </c>
-      <c r="H34" s="295" t="str">
+      <c r="H34" s="233" t="str">
         <f>I34</f>
         <v>148,5 MHz</v>
       </c>
-      <c r="I34" s="295" t="s">
+      <c r="I34" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J34" s="295" t="s">
+      <c r="J34" s="233" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D35" s="286">
+      <c r="D35" s="288">
         <v>32</v>
       </c>
-      <c r="E35" s="296" t="s">
+      <c r="E35" s="234" t="s">
         <v>901</v>
       </c>
       <c r="F35" s="222" t="s">
@@ -9327,19 +9385,19 @@
       <c r="G35" s="222">
         <v>20</v>
       </c>
-      <c r="H35" s="295" t="s">
+      <c r="H35" s="233" t="s">
         <v>909</v>
       </c>
-      <c r="I35" s="295" t="s">
+      <c r="I35" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J35" s="295" t="s">
+      <c r="J35" s="233" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D36" s="286"/>
-      <c r="E36" s="296" t="s">
+      <c r="D36" s="288"/>
+      <c r="E36" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F36" s="222" t="s">
@@ -9348,19 +9406,19 @@
       <c r="G36" s="222">
         <v>16</v>
       </c>
-      <c r="H36" s="295" t="s">
+      <c r="H36" s="233" t="s">
         <v>909</v>
       </c>
-      <c r="I36" s="295" t="s">
+      <c r="I36" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J36" s="295" t="s">
+      <c r="J36" s="233" t="s">
         <v>911</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="286"/>
-      <c r="E37" s="296" t="s">
+      <c r="D37" s="288"/>
+      <c r="E37" s="234" t="s">
         <v>901</v>
       </c>
       <c r="F37" s="222" t="s">
@@ -9369,20 +9427,20 @@
       <c r="G37" s="222">
         <v>40</v>
       </c>
-      <c r="H37" s="295" t="str">
+      <c r="H37" s="233" t="str">
         <f>I37</f>
         <v>148,5 MHz</v>
       </c>
-      <c r="I37" s="295" t="s">
+      <c r="I37" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J37" s="295" t="s">
+      <c r="J37" s="233" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D38" s="286"/>
-      <c r="E38" s="296" t="s">
+      <c r="D38" s="288"/>
+      <c r="E38" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F38" s="222" t="s">
@@ -9391,21 +9449,21 @@
       <c r="G38" s="222">
         <v>32</v>
       </c>
-      <c r="H38" s="292" t="s">
+      <c r="H38" s="230" t="s">
         <v>906</v>
       </c>
-      <c r="I38" s="295" t="s">
+      <c r="I38" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J38" s="295" t="s">
+      <c r="J38" s="233" t="s">
         <v>911</v>
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D39" s="286">
+      <c r="D39" s="288">
         <v>40</v>
       </c>
-      <c r="E39" s="296" t="s">
+      <c r="E39" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F39" s="222" t="s">
@@ -9414,19 +9472,19 @@
       <c r="G39" s="222">
         <v>20</v>
       </c>
-      <c r="H39" s="292" t="s">
+      <c r="H39" s="230" t="s">
         <v>909</v>
       </c>
-      <c r="I39" s="295" t="s">
+      <c r="I39" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J39" s="295" t="s">
+      <c r="J39" s="233" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D40" s="286"/>
-      <c r="E40" s="296" t="s">
+      <c r="D40" s="288"/>
+      <c r="E40" s="234" t="s">
         <v>902</v>
       </c>
       <c r="F40" s="222" t="s">
@@ -9435,19 +9493,19 @@
       <c r="G40" s="222">
         <v>40</v>
       </c>
-      <c r="H40" s="287" t="str">
+      <c r="H40" s="225" t="str">
         <f>I40</f>
         <v>148,5 MHz</v>
       </c>
-      <c r="I40" s="295" t="s">
+      <c r="I40" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J40" s="295" t="s">
+      <c r="J40" s="233" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D41" s="286">
+      <c r="D41" s="288">
         <v>64</v>
       </c>
       <c r="E41" s="222" t="s">
@@ -9459,18 +9517,18 @@
       <c r="G41" s="222">
         <v>40</v>
       </c>
-      <c r="H41" s="287" t="s">
+      <c r="H41" s="225" t="s">
         <v>909</v>
       </c>
-      <c r="I41" s="295" t="s">
+      <c r="I41" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J41" s="295" t="s">
+      <c r="J41" s="233" t="s">
         <v>912</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D42" s="286"/>
+      <c r="D42" s="288"/>
       <c r="E42" s="222" t="s">
         <v>902</v>
       </c>
@@ -9480,18 +9538,18 @@
       <c r="G42" s="222">
         <v>32</v>
       </c>
-      <c r="H42" s="287" t="s">
+      <c r="H42" s="225" t="s">
         <v>909</v>
       </c>
-      <c r="I42" s="295" t="s">
+      <c r="I42" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J42" s="295" t="s">
+      <c r="J42" s="233" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D43" s="289">
+      <c r="D43" s="227">
         <v>80</v>
       </c>
       <c r="E43" s="222" t="s">
@@ -9503,33 +9561,193 @@
       <c r="G43" s="222">
         <v>40</v>
       </c>
-      <c r="H43" s="287" t="s">
+      <c r="H43" s="225" t="s">
         <v>909</v>
       </c>
-      <c r="I43" s="295" t="s">
+      <c r="I43" s="233" t="s">
         <v>906</v>
       </c>
-      <c r="J43" s="295" t="s">
+      <c r="J43" s="233" t="s">
         <v>912</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="297" t="s">
+        <v>932</v>
+      </c>
+      <c r="D6" s="297"/>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>915</v>
+      </c>
+      <c r="D7">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>916</v>
+      </c>
+      <c r="D8">
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>917</v>
+      </c>
+      <c r="D9" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>918</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>919</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>920</v>
+      </c>
+      <c r="D12">
+        <f>D8</f>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>921</v>
+      </c>
+      <c r="D13">
+        <f>D8</f>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>922</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>923</v>
+      </c>
+      <c r="D15">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>924</v>
+      </c>
+      <c r="D16">
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>925</v>
+      </c>
+      <c r="D17" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>926</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>927</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>928</v>
+      </c>
+      <c r="D20">
+        <f>D16</f>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>929</v>
+      </c>
+      <c r="D21">
+        <f>D16</f>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>930</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9556,59 +9774,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="245" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="233"/>
-      <c r="E1" s="233"/>
-      <c r="F1" s="233"/>
-      <c r="G1" s="233"/>
-      <c r="H1" s="233"/>
-      <c r="I1" s="233"/>
-      <c r="J1" s="233"/>
-      <c r="K1" s="233"/>
-      <c r="L1" s="233"/>
-      <c r="M1" s="233"/>
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
     </row>
     <row r="2" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="233"/>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
+      <c r="A2" s="245"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="233"/>
-      <c r="B3" s="233"/>
-      <c r="C3" s="233"/>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
-      <c r="I3" s="233"/>
-      <c r="J3" s="233"/>
-      <c r="K3" s="233"/>
-      <c r="L3" s="233"/>
-      <c r="M3" s="233"/>
-      <c r="T3" s="224" t="s">
+      <c r="A3" s="245"/>
+      <c r="B3" s="245"/>
+      <c r="C3" s="245"/>
+      <c r="D3" s="245"/>
+      <c r="E3" s="245"/>
+      <c r="F3" s="245"/>
+      <c r="G3" s="245"/>
+      <c r="H3" s="245"/>
+      <c r="I3" s="245"/>
+      <c r="J3" s="245"/>
+      <c r="K3" s="245"/>
+      <c r="L3" s="245"/>
+      <c r="M3" s="245"/>
+      <c r="T3" s="236" t="s">
         <v>196</v>
       </c>
-      <c r="U3" s="225"/>
-      <c r="V3" s="225"/>
-      <c r="W3" s="225"/>
-      <c r="X3" s="225"/>
-      <c r="Y3" s="226"/>
+      <c r="U3" s="237"/>
+      <c r="V3" s="237"/>
+      <c r="W3" s="237"/>
+      <c r="X3" s="237"/>
+      <c r="Y3" s="238"/>
     </row>
     <row r="4" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -9899,14 +10117,14 @@
       <c r="M8" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="234" t="s">
+      <c r="T8" s="246" t="s">
         <v>200</v>
       </c>
-      <c r="U8" s="235"/>
-      <c r="V8" s="235"/>
-      <c r="W8" s="235"/>
-      <c r="X8" s="235"/>
-      <c r="Y8" s="236"/>
+      <c r="U8" s="247"/>
+      <c r="V8" s="247"/>
+      <c r="W8" s="247"/>
+      <c r="X8" s="247"/>
+      <c r="Y8" s="248"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
@@ -10989,22 +11207,22 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="224" t="s">
+      <c r="A39" s="236" t="s">
         <v>404</v>
       </c>
-      <c r="B39" s="225"/>
-      <c r="C39" s="225"/>
-      <c r="D39" s="225"/>
-      <c r="E39" s="225"/>
-      <c r="F39" s="226"/>
-      <c r="H39" s="230" t="s">
+      <c r="B39" s="237"/>
+      <c r="C39" s="237"/>
+      <c r="D39" s="237"/>
+      <c r="E39" s="237"/>
+      <c r="F39" s="238"/>
+      <c r="H39" s="242" t="s">
         <v>403</v>
       </c>
-      <c r="I39" s="231"/>
-      <c r="J39" s="231"/>
-      <c r="K39" s="231"/>
-      <c r="L39" s="231"/>
-      <c r="M39" s="232"/>
+      <c r="I39" s="243"/>
+      <c r="J39" s="243"/>
+      <c r="K39" s="243"/>
+      <c r="L39" s="243"/>
+      <c r="M39" s="244"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11041,52 +11259,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="235" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="243"/>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
-      <c r="K2" s="224" t="s">
+      <c r="A2" s="255"/>
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="255"/>
+      <c r="H2" s="255"/>
+      <c r="K2" s="236" t="s">
         <v>332</v>
       </c>
-      <c r="L2" s="225"/>
-      <c r="M2" s="225"/>
-      <c r="N2" s="225"/>
-      <c r="O2" s="226"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="238"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="259" t="s">
         <v>405</v>
       </c>
-      <c r="B3" s="248"/>
-      <c r="C3" s="248"/>
-      <c r="D3" s="248"/>
-      <c r="E3" s="248"/>
-      <c r="F3" s="248"/>
-      <c r="G3" s="248"/>
-      <c r="H3" s="249"/>
-      <c r="K3" s="244" t="s">
+      <c r="B3" s="260"/>
+      <c r="C3" s="260"/>
+      <c r="D3" s="260"/>
+      <c r="E3" s="260"/>
+      <c r="F3" s="260"/>
+      <c r="G3" s="260"/>
+      <c r="H3" s="261"/>
+      <c r="K3" s="256" t="s">
         <v>312</v>
       </c>
-      <c r="L3" s="245"/>
-      <c r="M3" s="245"/>
-      <c r="N3" s="245"/>
-      <c r="O3" s="246"/>
+      <c r="L3" s="257"/>
+      <c r="M3" s="257"/>
+      <c r="N3" s="257"/>
+      <c r="O3" s="258"/>
     </row>
     <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
@@ -11406,13 +11624,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K11" s="237" t="s">
+      <c r="K11" s="249" t="s">
         <v>317</v>
       </c>
-      <c r="L11" s="238"/>
-      <c r="M11" s="238"/>
-      <c r="N11" s="238"/>
-      <c r="O11" s="239"/>
+      <c r="L11" s="250"/>
+      <c r="M11" s="250"/>
+      <c r="N11" s="250"/>
+      <c r="O11" s="251"/>
     </row>
     <row r="12" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
@@ -11440,11 +11658,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K12" s="240"/>
-      <c r="L12" s="241"/>
-      <c r="M12" s="241"/>
-      <c r="N12" s="241"/>
-      <c r="O12" s="242"/>
+      <c r="K12" s="252"/>
+      <c r="L12" s="253"/>
+      <c r="M12" s="253"/>
+      <c r="N12" s="253"/>
+      <c r="O12" s="254"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
@@ -12752,52 +12970,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="235" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="251"/>
-      <c r="B2" s="251"/>
-      <c r="C2" s="251"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="K2" s="224" t="s">
+      <c r="A2" s="263"/>
+      <c r="B2" s="263"/>
+      <c r="C2" s="263"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
+      <c r="F2" s="263"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="K2" s="236" t="s">
         <v>425</v>
       </c>
-      <c r="L2" s="225"/>
-      <c r="M2" s="225"/>
-      <c r="N2" s="225"/>
-      <c r="O2" s="226"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="238"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="267" t="s">
         <v>402</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="256"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="256"/>
-      <c r="F3" s="256"/>
-      <c r="G3" s="256"/>
-      <c r="H3" s="257"/>
-      <c r="K3" s="252" t="s">
+      <c r="B3" s="268"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
+      <c r="H3" s="269"/>
+      <c r="K3" s="264" t="s">
         <v>426</v>
       </c>
-      <c r="L3" s="253"/>
-      <c r="M3" s="253"/>
-      <c r="N3" s="253"/>
-      <c r="O3" s="254"/>
+      <c r="L3" s="265"/>
+      <c r="M3" s="265"/>
+      <c r="N3" s="265"/>
+      <c r="O3" s="266"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="197" t="s">
@@ -13243,13 +13461,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K14" s="237" t="s">
+      <c r="K14" s="249" t="s">
         <v>317</v>
       </c>
-      <c r="L14" s="238"/>
-      <c r="M14" s="238"/>
-      <c r="N14" s="238"/>
-      <c r="O14" s="239"/>
+      <c r="L14" s="250"/>
+      <c r="M14" s="250"/>
+      <c r="N14" s="250"/>
+      <c r="O14" s="251"/>
     </row>
     <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
@@ -13277,11 +13495,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K15" s="240"/>
-      <c r="L15" s="241"/>
-      <c r="M15" s="241"/>
-      <c r="N15" s="241"/>
-      <c r="O15" s="242"/>
+      <c r="K15" s="252"/>
+      <c r="L15" s="253"/>
+      <c r="M15" s="253"/>
+      <c r="N15" s="253"/>
+      <c r="O15" s="254"/>
     </row>
     <row r="16" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
@@ -14468,16 +14686,16 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="250" t="s">
+      <c r="A55" s="262" t="s">
         <v>417</v>
       </c>
-      <c r="B55" s="250"/>
-      <c r="C55" s="250"/>
-      <c r="D55" s="250"/>
-      <c r="E55" s="250"/>
-      <c r="F55" s="250"/>
-      <c r="G55" s="250"/>
-      <c r="H55" s="250"/>
+      <c r="B55" s="262"/>
+      <c r="C55" s="262"/>
+      <c r="D55" s="262"/>
+      <c r="E55" s="262"/>
+      <c r="F55" s="262"/>
+      <c r="G55" s="262"/>
+      <c r="H55" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -14677,7 +14895,7 @@
       <c r="J8" s="158">
         <v>114</v>
       </c>
-      <c r="K8" s="263" t="s">
+      <c r="K8" s="275" t="s">
         <v>838</v>
       </c>
       <c r="L8" s="164"/>
@@ -14713,7 +14931,7 @@
       <c r="J9" s="158">
         <v>114</v>
       </c>
-      <c r="K9" s="263"/>
+      <c r="K9" s="275"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="181" t="s">
@@ -14862,7 +15080,7 @@
       <c r="J14" s="203">
         <v>19</v>
       </c>
-      <c r="K14" s="262" t="s">
+      <c r="K14" s="274" t="s">
         <v>838</v>
       </c>
     </row>
@@ -14897,7 +15115,7 @@
       <c r="J15" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="K15" s="262"/>
+      <c r="K15" s="274"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="181" t="s">
@@ -14930,7 +15148,7 @@
       <c r="J16" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="K16" s="262"/>
+      <c r="K16" s="274"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="181" t="s">
@@ -14961,7 +15179,7 @@
       <c r="J17" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="K17" s="262"/>
+      <c r="K17" s="274"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="181" t="s">
@@ -14992,18 +15210,18 @@
       <c r="J18" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="K18" s="262"/>
+      <c r="K18" s="274"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="260" t="s">
+      <c r="A19" s="272" t="s">
         <v>722</v>
       </c>
-      <c r="B19" s="261"/>
-      <c r="C19" s="261"/>
-      <c r="D19" s="261"/>
-      <c r="E19" s="261"/>
-      <c r="F19" s="261"/>
-      <c r="G19" s="261"/>
+      <c r="B19" s="273"/>
+      <c r="C19" s="273"/>
+      <c r="D19" s="273"/>
+      <c r="E19" s="273"/>
+      <c r="F19" s="273"/>
+      <c r="G19" s="273"/>
       <c r="H19" s="161"/>
       <c r="I19" s="161"/>
       <c r="J19" s="158"/>
@@ -15204,15 +15422,15 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="268" t="s">
+      <c r="A26" s="280" t="s">
         <v>729</v>
       </c>
-      <c r="B26" s="269"/>
-      <c r="C26" s="269"/>
-      <c r="D26" s="269"/>
-      <c r="E26" s="269"/>
-      <c r="F26" s="269"/>
-      <c r="G26" s="269"/>
+      <c r="B26" s="281"/>
+      <c r="C26" s="281"/>
+      <c r="D26" s="281"/>
+      <c r="E26" s="281"/>
+      <c r="F26" s="281"/>
+      <c r="G26" s="281"/>
       <c r="H26" s="161"/>
       <c r="I26" s="161"/>
       <c r="J26" s="158"/>
@@ -15248,15 +15466,15 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="264" t="s">
+      <c r="A28" s="276" t="s">
         <v>731</v>
       </c>
-      <c r="B28" s="265"/>
-      <c r="C28" s="265"/>
-      <c r="D28" s="265"/>
-      <c r="E28" s="265"/>
-      <c r="F28" s="265"/>
-      <c r="G28" s="265"/>
+      <c r="B28" s="277"/>
+      <c r="C28" s="277"/>
+      <c r="D28" s="277"/>
+      <c r="E28" s="277"/>
+      <c r="F28" s="277"/>
+      <c r="G28" s="277"/>
       <c r="H28" s="162"/>
       <c r="I28" s="162"/>
       <c r="J28" s="159"/>
@@ -15324,15 +15542,15 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="264" t="s">
+      <c r="A31" s="276" t="s">
         <v>734</v>
       </c>
-      <c r="B31" s="265"/>
-      <c r="C31" s="265"/>
-      <c r="D31" s="265"/>
-      <c r="E31" s="265"/>
-      <c r="F31" s="265"/>
-      <c r="G31" s="265"/>
+      <c r="B31" s="277"/>
+      <c r="C31" s="277"/>
+      <c r="D31" s="277"/>
+      <c r="E31" s="277"/>
+      <c r="F31" s="277"/>
+      <c r="G31" s="277"/>
       <c r="H31" s="162"/>
       <c r="I31" s="162"/>
       <c r="J31" s="159"/>
@@ -15402,15 +15620,15 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="264" t="s">
+      <c r="A34" s="276" t="s">
         <v>737</v>
       </c>
-      <c r="B34" s="265"/>
-      <c r="C34" s="265"/>
-      <c r="D34" s="265"/>
-      <c r="E34" s="265"/>
-      <c r="F34" s="265"/>
-      <c r="G34" s="265"/>
+      <c r="B34" s="277"/>
+      <c r="C34" s="277"/>
+      <c r="D34" s="277"/>
+      <c r="E34" s="277"/>
+      <c r="F34" s="277"/>
+      <c r="G34" s="277"/>
       <c r="H34" s="162"/>
       <c r="I34" s="162"/>
       <c r="J34" s="159"/>
@@ -15446,15 +15664,15 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="264" t="s">
+      <c r="A36" s="276" t="s">
         <v>740</v>
       </c>
-      <c r="B36" s="265"/>
-      <c r="C36" s="265"/>
-      <c r="D36" s="265"/>
-      <c r="E36" s="265"/>
-      <c r="F36" s="265"/>
-      <c r="G36" s="265"/>
+      <c r="B36" s="277"/>
+      <c r="C36" s="277"/>
+      <c r="D36" s="277"/>
+      <c r="E36" s="277"/>
+      <c r="F36" s="277"/>
+      <c r="G36" s="277"/>
       <c r="H36" s="162"/>
       <c r="I36" s="162"/>
       <c r="J36" s="159"/>
@@ -15520,15 +15738,15 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="266" t="s">
+      <c r="A39" s="278" t="s">
         <v>742</v>
       </c>
-      <c r="B39" s="267"/>
-      <c r="C39" s="267"/>
-      <c r="D39" s="267"/>
-      <c r="E39" s="267"/>
-      <c r="F39" s="267"/>
-      <c r="G39" s="267"/>
+      <c r="B39" s="279"/>
+      <c r="C39" s="279"/>
+      <c r="D39" s="279"/>
+      <c r="E39" s="279"/>
+      <c r="F39" s="279"/>
+      <c r="G39" s="279"/>
       <c r="H39" s="162"/>
       <c r="I39" s="162"/>
       <c r="J39" s="159"/>
@@ -15628,15 +15846,15 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="264" t="s">
+      <c r="A43" s="276" t="s">
         <v>746</v>
       </c>
-      <c r="B43" s="265"/>
-      <c r="C43" s="265"/>
-      <c r="D43" s="265"/>
-      <c r="E43" s="265"/>
-      <c r="F43" s="265"/>
-      <c r="G43" s="265"/>
+      <c r="B43" s="277"/>
+      <c r="C43" s="277"/>
+      <c r="D43" s="277"/>
+      <c r="E43" s="277"/>
+      <c r="F43" s="277"/>
+      <c r="G43" s="277"/>
       <c r="H43" s="162"/>
       <c r="I43" s="162"/>
       <c r="J43" s="159"/>
@@ -15734,15 +15952,15 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="260" t="s">
+      <c r="A47" s="272" t="s">
         <v>750</v>
       </c>
-      <c r="B47" s="261"/>
-      <c r="C47" s="261"/>
-      <c r="D47" s="261"/>
-      <c r="E47" s="261"/>
-      <c r="F47" s="261"/>
-      <c r="G47" s="261"/>
+      <c r="B47" s="273"/>
+      <c r="C47" s="273"/>
+      <c r="D47" s="273"/>
+      <c r="E47" s="273"/>
+      <c r="F47" s="273"/>
+      <c r="G47" s="273"/>
       <c r="H47" s="163"/>
       <c r="I47" s="163"/>
       <c r="J47" s="160"/>
@@ -15812,15 +16030,15 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="258" t="s">
+      <c r="A50" s="270" t="s">
         <v>754</v>
       </c>
-      <c r="B50" s="259"/>
-      <c r="C50" s="259"/>
-      <c r="D50" s="259"/>
-      <c r="E50" s="259"/>
-      <c r="F50" s="259"/>
-      <c r="G50" s="259"/>
+      <c r="B50" s="271"/>
+      <c r="C50" s="271"/>
+      <c r="D50" s="271"/>
+      <c r="E50" s="271"/>
+      <c r="F50" s="271"/>
+      <c r="G50" s="271"/>
       <c r="H50" s="163"/>
       <c r="I50" s="163"/>
       <c r="J50" s="160"/>
@@ -15858,15 +16076,15 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="258" t="s">
+      <c r="A52" s="270" t="s">
         <v>755</v>
       </c>
-      <c r="B52" s="259"/>
-      <c r="C52" s="259"/>
-      <c r="D52" s="259"/>
-      <c r="E52" s="259"/>
-      <c r="F52" s="259"/>
-      <c r="G52" s="259"/>
+      <c r="B52" s="271"/>
+      <c r="C52" s="271"/>
+      <c r="D52" s="271"/>
+      <c r="E52" s="271"/>
+      <c r="F52" s="271"/>
+      <c r="G52" s="271"/>
       <c r="H52" s="163"/>
       <c r="I52" s="163"/>
       <c r="J52" s="160"/>
@@ -15936,15 +16154,15 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="258" t="s">
+      <c r="A55" s="270" t="s">
         <v>759</v>
       </c>
-      <c r="B55" s="259"/>
-      <c r="C55" s="259"/>
-      <c r="D55" s="259"/>
-      <c r="E55" s="259"/>
-      <c r="F55" s="259"/>
-      <c r="G55" s="259"/>
+      <c r="B55" s="271"/>
+      <c r="C55" s="271"/>
+      <c r="D55" s="271"/>
+      <c r="E55" s="271"/>
+      <c r="F55" s="271"/>
+      <c r="G55" s="271"/>
       <c r="H55" s="163"/>
       <c r="I55" s="163"/>
       <c r="J55" s="160"/>
@@ -15998,15 +16216,15 @@
       <c r="J57" s="49"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="258" t="s">
+      <c r="A58" s="270" t="s">
         <v>762</v>
       </c>
-      <c r="B58" s="259"/>
-      <c r="C58" s="259"/>
-      <c r="D58" s="259"/>
-      <c r="E58" s="259"/>
-      <c r="F58" s="259"/>
-      <c r="G58" s="259"/>
+      <c r="B58" s="271"/>
+      <c r="C58" s="271"/>
+      <c r="D58" s="271"/>
+      <c r="E58" s="271"/>
+      <c r="F58" s="271"/>
+      <c r="G58" s="271"/>
       <c r="H58" s="163"/>
       <c r="I58" s="163"/>
       <c r="J58" s="160"/>
@@ -16044,15 +16262,15 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="260" t="s">
+      <c r="A60" s="272" t="s">
         <v>764</v>
       </c>
-      <c r="B60" s="261"/>
-      <c r="C60" s="261"/>
-      <c r="D60" s="261"/>
-      <c r="E60" s="261"/>
-      <c r="F60" s="261"/>
-      <c r="G60" s="261"/>
+      <c r="B60" s="273"/>
+      <c r="C60" s="273"/>
+      <c r="D60" s="273"/>
+      <c r="E60" s="273"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="273"/>
       <c r="H60" s="161"/>
       <c r="I60" s="161"/>
       <c r="J60" s="158"/>
@@ -16226,15 +16444,15 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="260" t="s">
+      <c r="A67" s="272" t="s">
         <v>771</v>
       </c>
-      <c r="B67" s="261"/>
-      <c r="C67" s="261"/>
-      <c r="D67" s="261"/>
-      <c r="E67" s="261"/>
-      <c r="F67" s="261"/>
-      <c r="G67" s="261"/>
+      <c r="B67" s="273"/>
+      <c r="C67" s="273"/>
+      <c r="D67" s="273"/>
+      <c r="E67" s="273"/>
+      <c r="F67" s="273"/>
+      <c r="G67" s="273"/>
       <c r="H67" s="161"/>
       <c r="I67" s="161"/>
       <c r="J67" s="158"/>
@@ -16461,11 +16679,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="K14:K18"/>
-    <mergeCell ref="K8:K9"/>
     <mergeCell ref="A67:G67"/>
     <mergeCell ref="A36:G36"/>
     <mergeCell ref="A39:G39"/>
@@ -16478,6 +16691,11 @@
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="K14:K18"/>
+    <mergeCell ref="K8:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17955,17 +18173,17 @@
       <c r="K50" s="58"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="255" t="s">
+      <c r="A54" s="267" t="s">
         <v>402</v>
       </c>
-      <c r="B54" s="256"/>
-      <c r="C54" s="256"/>
-      <c r="D54" s="256"/>
-      <c r="E54" s="256"/>
-      <c r="F54" s="256"/>
-      <c r="G54" s="256"/>
-      <c r="H54" s="256"/>
-      <c r="I54" s="257"/>
+      <c r="B54" s="268"/>
+      <c r="C54" s="268"/>
+      <c r="D54" s="268"/>
+      <c r="E54" s="268"/>
+      <c r="F54" s="268"/>
+      <c r="G54" s="268"/>
+      <c r="H54" s="268"/>
+      <c r="I54" s="269"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="197" t="s">
@@ -19292,11 +19510,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="270" t="s">
+      <c r="A2" s="282" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="271"/>
-      <c r="C2" s="272"/>
+      <c r="B2" s="283"/>
+      <c r="C2" s="284"/>
     </row>
     <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -19398,19 +19616,19 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="270" t="s">
+      <c r="A12" s="282" t="s">
         <v>359</v>
       </c>
-      <c r="B12" s="271"/>
-      <c r="C12" s="272"/>
+      <c r="B12" s="283"/>
+      <c r="C12" s="284"/>
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="270" t="s">
+      <c r="A15" s="282" t="s">
         <v>361</v>
       </c>
-      <c r="B15" s="271"/>
-      <c r="C15" s="272"/>
+      <c r="B15" s="283"/>
+      <c r="C15" s="284"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
@@ -19512,19 +19730,19 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="270" t="s">
+      <c r="A25" s="282" t="s">
         <v>359</v>
       </c>
-      <c r="B25" s="271"/>
-      <c r="C25" s="272"/>
+      <c r="B25" s="283"/>
+      <c r="C25" s="284"/>
     </row>
     <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="270" t="s">
+      <c r="A28" s="282" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="271"/>
-      <c r="C28" s="272"/>
+      <c r="B28" s="283"/>
+      <c r="C28" s="284"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
@@ -19624,11 +19842,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="270" t="s">
+      <c r="A38" s="282" t="s">
         <v>359</v>
       </c>
-      <c r="B38" s="271"/>
-      <c r="C38" s="272"/>
+      <c r="B38" s="283"/>
+      <c r="C38" s="284"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -22186,7 +22404,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="273" t="s">
+      <c r="G107" s="285" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -22222,7 +22440,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="274"/>
+      <c r="G108" s="286"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -22260,7 +22478,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="275" t="s">
+      <c r="J109" s="287" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -22282,7 +22500,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="275"/>
+      <c r="J110" s="287"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -22302,7 +22520,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="275"/>
+      <c r="J111" s="287"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -22322,7 +22540,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="275"/>
+      <c r="J112" s="287"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
dia 22 - noite
</commit_message>
<xml_diff>
--- a/mieec-distrib-v2014/outras_cenas/Book1.xlsx
+++ b/mieec-distrib-v2014/outras_cenas/Book1.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="792">
   <si>
     <t>I/O</t>
   </si>
@@ -2408,6 +2408,15 @@
   </si>
   <si>
     <t>R40</t>
+  </si>
+  <si>
+    <t>clk_px_in</t>
+  </si>
+  <si>
+    <t>pixel_in [0] a pixel_in [29]</t>
+  </si>
+  <si>
+    <t>14 e 15</t>
   </si>
 </sst>
 </file>
@@ -3329,7 +3338,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3361,8 +3370,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3857,6 +3870,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4010,8 +4029,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -4029,6 +4051,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
@@ -4040,6 +4064,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -4335,60 +4361,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="188" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
-      <c r="M1" s="186"/>
-      <c r="N1" s="186"/>
-      <c r="O1" s="186"/>
-      <c r="P1" s="186"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
+      <c r="M1" s="188"/>
+      <c r="N1" s="188"/>
+      <c r="O1" s="188"/>
+      <c r="P1" s="188"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
-      <c r="J2" s="186"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="186"/>
-      <c r="M2" s="186"/>
-      <c r="N2" s="186"/>
-      <c r="O2" s="186"/>
-      <c r="P2" s="186"/>
+      <c r="A2" s="188"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
+      <c r="K2" s="188"/>
+      <c r="L2" s="188"/>
+      <c r="M2" s="188"/>
+      <c r="N2" s="188"/>
+      <c r="O2" s="188"/>
+      <c r="P2" s="188"/>
     </row>
     <row r="3" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="186"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="186"/>
-      <c r="M3" s="186"/>
-      <c r="N3" s="186"/>
-      <c r="O3" s="186"/>
-      <c r="P3" s="186"/>
+      <c r="A3" s="188"/>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="188"/>
+      <c r="L3" s="188"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
+      <c r="O3" s="188"/>
+      <c r="P3" s="188"/>
     </row>
     <row r="4" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -4421,14 +4447,14 @@
       <c r="K4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="189" t="s">
         <v>196</v>
       </c>
-      <c r="N4" s="188"/>
-      <c r="O4" s="188"/>
-      <c r="P4" s="188"/>
-      <c r="Q4" s="188"/>
-      <c r="R4" s="189"/>
+      <c r="N4" s="190"/>
+      <c r="O4" s="190"/>
+      <c r="P4" s="190"/>
+      <c r="Q4" s="190"/>
+      <c r="R4" s="191"/>
     </row>
     <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4649,14 +4675,14 @@
       <c r="F9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="190" t="s">
+      <c r="M9" s="192" t="s">
         <v>200</v>
       </c>
-      <c r="N9" s="191"/>
-      <c r="O9" s="191"/>
-      <c r="P9" s="191"/>
-      <c r="Q9" s="191"/>
-      <c r="R9" s="192"/>
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="194"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -5239,14 +5265,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="193" t="s">
+      <c r="A39" s="195" t="s">
         <v>403</v>
       </c>
-      <c r="B39" s="194"/>
-      <c r="C39" s="194"/>
-      <c r="D39" s="194"/>
-      <c r="E39" s="194"/>
-      <c r="F39" s="195"/>
+      <c r="B39" s="196"/>
+      <c r="C39" s="196"/>
+      <c r="D39" s="196"/>
+      <c r="E39" s="196"/>
+      <c r="F39" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5323,10 +5349,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="230" t="s">
         <v>703</v>
       </c>
-      <c r="D6" s="235">
+      <c r="D6" s="237">
         <v>64</v>
       </c>
       <c r="E6" s="46">
@@ -5355,8 +5381,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C7" s="229"/>
-      <c r="D7" s="232"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="234"/>
       <c r="E7" s="92">
         <v>1</v>
       </c>
@@ -5383,13 +5409,13 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="230" t="s">
+      <c r="C8" s="232" t="s">
         <v>704</v>
       </c>
-      <c r="D8" s="227">
+      <c r="D8" s="229">
         <v>40</v>
       </c>
-      <c r="E8" s="227">
+      <c r="E8" s="229">
         <v>0</v>
       </c>
       <c r="F8" s="67">
@@ -5415,9 +5441,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="230"/>
-      <c r="D9" s="227"/>
-      <c r="E9" s="227"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="229"/>
+      <c r="E9" s="229"/>
       <c r="F9" s="92">
         <v>1</v>
       </c>
@@ -5441,10 +5467,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="230" t="s">
+      <c r="C10" s="232" t="s">
         <v>705</v>
       </c>
-      <c r="D10" s="232">
+      <c r="D10" s="234">
         <v>16</v>
       </c>
       <c r="E10" s="92">
@@ -5473,8 +5499,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="234"/>
-      <c r="D11" s="233"/>
+      <c r="C11" s="236"/>
+      <c r="D11" s="235"/>
       <c r="E11" s="57">
         <v>0</v>
       </c>
@@ -5545,7 +5571,7 @@
       <c r="K14" s="143"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="231">
+      <c r="D15" s="233">
         <v>16</v>
       </c>
       <c r="E15" s="179" t="s">
@@ -5571,7 +5597,7 @@
       <c r="K15" s="143"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="231"/>
+      <c r="D16" s="233"/>
       <c r="E16" s="179" t="s">
         <v>734</v>
       </c>
@@ -5621,7 +5647,7 @@
       <c r="K17" s="143"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D18" s="231">
+      <c r="D18" s="233">
         <v>32</v>
       </c>
       <c r="E18" s="179" t="s">
@@ -5647,7 +5673,7 @@
       <c r="K18" s="143"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D19" s="231"/>
+      <c r="D19" s="233"/>
       <c r="E19" s="180" t="s">
         <v>734</v>
       </c>
@@ -5671,7 +5697,7 @@
       <c r="K19" s="143"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="231"/>
+      <c r="D20" s="233"/>
       <c r="E20" s="180" t="s">
         <v>733</v>
       </c>
@@ -5695,7 +5721,7 @@
       <c r="K20" s="143"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D21" s="231"/>
+      <c r="D21" s="233"/>
       <c r="E21" s="180" t="s">
         <v>734</v>
       </c>
@@ -5718,7 +5744,7 @@
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="231">
+      <c r="D22" s="233">
         <v>40</v>
       </c>
       <c r="E22" s="180" t="s">
@@ -5743,7 +5769,7 @@
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D23" s="231"/>
+      <c r="D23" s="233"/>
       <c r="E23" s="180" t="s">
         <v>734</v>
       </c>
@@ -5767,7 +5793,7 @@
       <c r="K23" s="179"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D24" s="231">
+      <c r="D24" s="233">
         <v>64</v>
       </c>
       <c r="E24" s="173" t="s">
@@ -5792,7 +5818,7 @@
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="231"/>
+      <c r="D25" s="233"/>
       <c r="E25" s="173" t="s">
         <v>734</v>
       </c>
@@ -5868,7 +5894,7 @@
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D32" s="231">
+      <c r="D32" s="233">
         <v>16</v>
       </c>
       <c r="E32" s="185" t="s">
@@ -5892,7 +5918,7 @@
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D33" s="231"/>
+      <c r="D33" s="233"/>
       <c r="E33" s="185" t="s">
         <v>734</v>
       </c>
@@ -5938,7 +5964,7 @@
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D35" s="231">
+      <c r="D35" s="233">
         <v>32</v>
       </c>
       <c r="E35" s="185" t="s">
@@ -5961,7 +5987,7 @@
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D36" s="231"/>
+      <c r="D36" s="233"/>
       <c r="E36" s="185" t="s">
         <v>734</v>
       </c>
@@ -5982,7 +6008,7 @@
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D37" s="231"/>
+      <c r="D37" s="233"/>
       <c r="E37" s="185" t="s">
         <v>733</v>
       </c>
@@ -6004,7 +6030,7 @@
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D38" s="231"/>
+      <c r="D38" s="233"/>
       <c r="E38" s="185" t="s">
         <v>734</v>
       </c>
@@ -6025,7 +6051,7 @@
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D39" s="231">
+      <c r="D39" s="233">
         <v>40</v>
       </c>
       <c r="E39" s="185" t="s">
@@ -6048,7 +6074,7 @@
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D40" s="231"/>
+      <c r="D40" s="233"/>
       <c r="E40" s="185" t="s">
         <v>734</v>
       </c>
@@ -6070,7 +6096,7 @@
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D41" s="231">
+      <c r="D41" s="233">
         <v>64</v>
       </c>
       <c r="E41" s="173" t="s">
@@ -6093,7 +6119,7 @@
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D42" s="231"/>
+      <c r="D42" s="233"/>
       <c r="E42" s="173" t="s">
         <v>734</v>
       </c>
@@ -6173,10 +6199,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="236" t="s">
+      <c r="C6" s="238" t="s">
         <v>764</v>
       </c>
-      <c r="D6" s="236"/>
+      <c r="D6" s="238"/>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
@@ -6320,15 +6346,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E26"/>
+  <dimension ref="B4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6457,197 +6483,315 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="C13" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="D13" t="s">
-        <v>715</v>
+        <v>148</v>
       </c>
       <c r="E13">
-        <v>114</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="C14" t="s">
-        <v>777</v>
+        <v>532</v>
       </c>
       <c r="D14" t="s">
-        <v>716</v>
+        <v>149</v>
       </c>
       <c r="E14">
-        <v>114</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="C15" t="s">
-        <v>780</v>
+        <v>531</v>
       </c>
       <c r="D15" t="s">
-        <v>684</v>
+        <v>151</v>
       </c>
       <c r="E15">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="C16" t="s">
-        <v>781</v>
+        <v>530</v>
       </c>
       <c r="D16" t="s">
-        <v>708</v>
+        <v>150</v>
       </c>
       <c r="E16">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="C17" t="s">
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="D17" t="s">
-        <v>707</v>
-      </c>
-      <c r="E17">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+        <v>770</v>
+      </c>
+      <c r="E17" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>772</v>
       </c>
       <c r="C18" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="D18" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="E18">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>772</v>
       </c>
       <c r="C19" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="D19" t="s">
-        <v>787</v>
+        <v>716</v>
       </c>
       <c r="E19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>772</v>
       </c>
       <c r="C20" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="D20" t="s">
-        <v>788</v>
+        <v>684</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>772</v>
       </c>
       <c r="C21" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="D21" t="s">
-        <v>779</v>
+        <v>708</v>
       </c>
       <c r="E21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>772</v>
       </c>
       <c r="C22" t="s">
-        <v>768</v>
+        <v>782</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>707</v>
       </c>
       <c r="E22">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>772</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>783</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>709</v>
       </c>
       <c r="E23">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H23" s="187" t="s">
+        <v>533</v>
+      </c>
+      <c r="I23" s="187" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="109" t="s">
+        <v>148</v>
+      </c>
+      <c r="K23" s="187">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>772</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>784</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>787</v>
       </c>
       <c r="E24">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H24" s="186" t="s">
+        <v>530</v>
+      </c>
+      <c r="I24" s="186" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" s="186">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>772</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>785</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>788</v>
       </c>
       <c r="E25">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H25" s="186" t="s">
+        <v>531</v>
+      </c>
+      <c r="I25" s="186" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="K25" s="186">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>772</v>
       </c>
       <c r="C26" t="s">
+        <v>778</v>
+      </c>
+      <c r="D26" t="s">
+        <v>779</v>
+      </c>
+      <c r="E26">
+        <v>19</v>
+      </c>
+      <c r="H26" s="186" t="s">
+        <v>532</v>
+      </c>
+      <c r="I26" s="186" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="K26" s="51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>772</v>
+      </c>
+      <c r="C27" t="s">
+        <v>768</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>772</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>772</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>772</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>772</v>
+      </c>
+      <c r="C31" t="s">
         <v>769</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D31" t="s">
         <v>770</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E31" s="239" t="s">
         <v>771</v>
       </c>
     </row>
@@ -6677,59 +6821,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="198" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="196"/>
-      <c r="I1" s="196"/>
-      <c r="J1" s="196"/>
-      <c r="K1" s="196"/>
-      <c r="L1" s="196"/>
-      <c r="M1" s="196"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
     </row>
     <row r="2" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
+      <c r="A2" s="198"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="196"/>
-      <c r="B3" s="196"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="196"/>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="196"/>
-      <c r="M3" s="196"/>
-      <c r="T3" s="187" t="s">
+      <c r="A3" s="198"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
+      <c r="J3" s="198"/>
+      <c r="K3" s="198"/>
+      <c r="L3" s="198"/>
+      <c r="M3" s="198"/>
+      <c r="T3" s="189" t="s">
         <v>196</v>
       </c>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="189"/>
+      <c r="U3" s="190"/>
+      <c r="V3" s="190"/>
+      <c r="W3" s="190"/>
+      <c r="X3" s="190"/>
+      <c r="Y3" s="191"/>
     </row>
     <row r="4" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -7020,14 +7164,14 @@
       <c r="M8" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="197" t="s">
+      <c r="T8" s="199" t="s">
         <v>200</v>
       </c>
-      <c r="U8" s="198"/>
-      <c r="V8" s="198"/>
-      <c r="W8" s="198"/>
-      <c r="X8" s="198"/>
-      <c r="Y8" s="199"/>
+      <c r="U8" s="200"/>
+      <c r="V8" s="200"/>
+      <c r="W8" s="200"/>
+      <c r="X8" s="200"/>
+      <c r="Y8" s="201"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
@@ -8110,22 +8254,22 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="187" t="s">
+      <c r="A39" s="189" t="s">
         <v>404</v>
       </c>
-      <c r="B39" s="188"/>
-      <c r="C39" s="188"/>
-      <c r="D39" s="188"/>
-      <c r="E39" s="188"/>
-      <c r="F39" s="189"/>
-      <c r="H39" s="193" t="s">
+      <c r="B39" s="190"/>
+      <c r="C39" s="190"/>
+      <c r="D39" s="190"/>
+      <c r="E39" s="190"/>
+      <c r="F39" s="191"/>
+      <c r="H39" s="195" t="s">
         <v>403</v>
       </c>
-      <c r="I39" s="194"/>
-      <c r="J39" s="194"/>
-      <c r="K39" s="194"/>
-      <c r="L39" s="194"/>
-      <c r="M39" s="195"/>
+      <c r="I39" s="196"/>
+      <c r="J39" s="196"/>
+      <c r="K39" s="196"/>
+      <c r="L39" s="196"/>
+      <c r="M39" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8143,8 +8287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8162,52 +8306,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="188" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="206"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="206"/>
-      <c r="F2" s="206"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="206"/>
-      <c r="K2" s="187" t="s">
+      <c r="A2" s="208"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208"/>
+      <c r="K2" s="189" t="s">
         <v>332</v>
       </c>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="189"/>
+      <c r="L2" s="190"/>
+      <c r="M2" s="190"/>
+      <c r="N2" s="190"/>
+      <c r="O2" s="191"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="210" t="s">
+      <c r="A3" s="212" t="s">
         <v>405</v>
       </c>
-      <c r="B3" s="211"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
-      <c r="H3" s="212"/>
-      <c r="K3" s="207" t="s">
+      <c r="B3" s="213"/>
+      <c r="C3" s="213"/>
+      <c r="D3" s="213"/>
+      <c r="E3" s="213"/>
+      <c r="F3" s="213"/>
+      <c r="G3" s="213"/>
+      <c r="H3" s="214"/>
+      <c r="K3" s="209" t="s">
         <v>312</v>
       </c>
-      <c r="L3" s="208"/>
-      <c r="M3" s="208"/>
-      <c r="N3" s="208"/>
-      <c r="O3" s="209"/>
+      <c r="L3" s="210"/>
+      <c r="M3" s="210"/>
+      <c r="N3" s="210"/>
+      <c r="O3" s="211"/>
     </row>
     <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
@@ -8527,13 +8671,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K11" s="200" t="s">
+      <c r="K11" s="202" t="s">
         <v>317</v>
       </c>
-      <c r="L11" s="201"/>
-      <c r="M11" s="201"/>
-      <c r="N11" s="201"/>
-      <c r="O11" s="202"/>
+      <c r="L11" s="203"/>
+      <c r="M11" s="203"/>
+      <c r="N11" s="203"/>
+      <c r="O11" s="204"/>
     </row>
     <row r="12" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
@@ -8561,11 +8705,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS18</v>
       </c>
-      <c r="K12" s="203"/>
-      <c r="L12" s="204"/>
-      <c r="M12" s="204"/>
-      <c r="N12" s="204"/>
-      <c r="O12" s="205"/>
+      <c r="K12" s="205"/>
+      <c r="L12" s="206"/>
+      <c r="M12" s="206"/>
+      <c r="N12" s="206"/>
+      <c r="O12" s="207"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
@@ -9873,52 +10017,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="188" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="K2" s="187" t="s">
+      <c r="A2" s="216"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="K2" s="189" t="s">
         <v>425</v>
       </c>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="189"/>
+      <c r="L2" s="190"/>
+      <c r="M2" s="190"/>
+      <c r="N2" s="190"/>
+      <c r="O2" s="191"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="220" t="s">
         <v>402</v>
       </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="219"/>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="220"/>
-      <c r="K3" s="215" t="s">
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="222"/>
+      <c r="K3" s="217" t="s">
         <v>426</v>
       </c>
-      <c r="L3" s="216"/>
-      <c r="M3" s="216"/>
-      <c r="N3" s="216"/>
-      <c r="O3" s="217"/>
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218"/>
+      <c r="O3" s="219"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="157" t="s">
@@ -10364,13 +10508,13 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K14" s="200" t="s">
+      <c r="K14" s="202" t="s">
         <v>317</v>
       </c>
-      <c r="L14" s="201"/>
-      <c r="M14" s="201"/>
-      <c r="N14" s="201"/>
-      <c r="O14" s="202"/>
+      <c r="L14" s="203"/>
+      <c r="M14" s="203"/>
+      <c r="N14" s="203"/>
+      <c r="O14" s="204"/>
     </row>
     <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
@@ -10398,11 +10542,11 @@
         <f t="shared" si="0"/>
         <v>LVCMOS25</v>
       </c>
-      <c r="K15" s="203"/>
-      <c r="L15" s="204"/>
-      <c r="M15" s="204"/>
-      <c r="N15" s="204"/>
-      <c r="O15" s="205"/>
+      <c r="K15" s="205"/>
+      <c r="L15" s="206"/>
+      <c r="M15" s="206"/>
+      <c r="N15" s="206"/>
+      <c r="O15" s="207"/>
     </row>
     <row r="16" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
@@ -11589,16 +11733,16 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="213" t="s">
+      <c r="A55" s="215" t="s">
         <v>417</v>
       </c>
-      <c r="B55" s="213"/>
-      <c r="C55" s="213"/>
-      <c r="D55" s="213"/>
-      <c r="E55" s="213"/>
-      <c r="F55" s="213"/>
-      <c r="G55" s="213"/>
-      <c r="H55" s="213"/>
+      <c r="B55" s="215"/>
+      <c r="C55" s="215"/>
+      <c r="D55" s="215"/>
+      <c r="E55" s="215"/>
+      <c r="F55" s="215"/>
+      <c r="G55" s="215"/>
+      <c r="H55" s="215"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -13086,17 +13230,17 @@
       <c r="K50" s="58"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="218" t="s">
+      <c r="A54" s="220" t="s">
         <v>402</v>
       </c>
-      <c r="B54" s="219"/>
-      <c r="C54" s="219"/>
-      <c r="D54" s="219"/>
-      <c r="E54" s="219"/>
-      <c r="F54" s="219"/>
-      <c r="G54" s="219"/>
-      <c r="H54" s="219"/>
-      <c r="I54" s="220"/>
+      <c r="B54" s="221"/>
+      <c r="C54" s="221"/>
+      <c r="D54" s="221"/>
+      <c r="E54" s="221"/>
+      <c r="F54" s="221"/>
+      <c r="G54" s="221"/>
+      <c r="H54" s="221"/>
+      <c r="I54" s="222"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="157" t="s">
@@ -14423,11 +14567,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="223" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="223"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="225"/>
     </row>
     <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -14529,19 +14673,19 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="221" t="s">
+      <c r="A12" s="223" t="s">
         <v>359</v>
       </c>
-      <c r="B12" s="222"/>
-      <c r="C12" s="223"/>
+      <c r="B12" s="224"/>
+      <c r="C12" s="225"/>
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="221" t="s">
+      <c r="A15" s="223" t="s">
         <v>361</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="C15" s="223"/>
+      <c r="B15" s="224"/>
+      <c r="C15" s="225"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
@@ -14643,19 +14787,19 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="221" t="s">
+      <c r="A25" s="223" t="s">
         <v>359</v>
       </c>
-      <c r="B25" s="222"/>
-      <c r="C25" s="223"/>
+      <c r="B25" s="224"/>
+      <c r="C25" s="225"/>
     </row>
     <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="221" t="s">
+      <c r="A28" s="223" t="s">
         <v>361</v>
       </c>
-      <c r="B28" s="222"/>
-      <c r="C28" s="223"/>
+      <c r="B28" s="224"/>
+      <c r="C28" s="225"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
@@ -14755,11 +14899,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="221" t="s">
+      <c r="A38" s="223" t="s">
         <v>359</v>
       </c>
-      <c r="B38" s="222"/>
-      <c r="C38" s="223"/>
+      <c r="B38" s="224"/>
+      <c r="C38" s="225"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17317,7 +17461,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="224" t="s">
+      <c r="G107" s="226" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -17353,7 +17497,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="225"/>
+      <c r="G108" s="227"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -17391,7 +17535,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="226" t="s">
+      <c r="J109" s="228" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -17413,7 +17557,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="226"/>
+      <c r="J110" s="228"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -17433,7 +17577,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="226"/>
+      <c r="J111" s="228"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -17453,7 +17597,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="226"/>
+      <c r="J112" s="228"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>
@@ -20056,7 +20200,7 @@
       <c r="F107" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="G107" s="224" t="s">
+      <c r="G107" s="226" t="s">
         <v>686</v>
       </c>
       <c r="H107" s="101"/>
@@ -20092,7 +20236,7 @@
       <c r="F108" s="117" t="s">
         <v>607</v>
       </c>
-      <c r="G108" s="225"/>
+      <c r="G108" s="227"/>
       <c r="H108" s="49"/>
       <c r="J108" t="s">
         <v>195</v>
@@ -20130,7 +20274,7 @@
         <v>685</v>
       </c>
       <c r="H109" s="58"/>
-      <c r="J109" s="226" t="s">
+      <c r="J109" s="228" t="s">
         <v>194</v>
       </c>
       <c r="K109" t="s">
@@ -20158,7 +20302,7 @@
       <c r="F110" s="116"/>
       <c r="G110"/>
       <c r="H110"/>
-      <c r="J110" s="226"/>
+      <c r="J110" s="228"/>
       <c r="K110" t="s">
         <v>195</v>
       </c>
@@ -20178,7 +20322,7 @@
       <c r="F111" s="116"/>
       <c r="G111"/>
       <c r="H111"/>
-      <c r="J111" s="226"/>
+      <c r="J111" s="228"/>
       <c r="K111" t="s">
         <v>194</v>
       </c>
@@ -20198,7 +20342,7 @@
       <c r="F112" s="116"/>
       <c r="G112"/>
       <c r="H112"/>
-      <c r="J112" s="226"/>
+      <c r="J112" s="228"/>
       <c r="K112" t="s">
         <v>194</v>
       </c>

</xml_diff>